<commit_message>
Notebook for CERRO DOMINADOR
two escenarios explored
</commit_message>
<xml_diff>
--- a/Precio_Medio_de_Mercado.xlsx
+++ b/Precio_Medio_de_Mercado.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmaldonado\Documents\11 PMM\155 PMM Publicado en ENE 2020\02 Archivos Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Documents/GitKraken/CSP_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A09FC1-0BDD-1448-B42D-8274A1F74AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="645" windowWidth="26700" windowHeight="11190" tabRatio="455"/>
+    <workbookView xWindow="2100" yWindow="640" windowWidth="26700" windowHeight="11200" tabRatio="455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMM SEN" sheetId="3" r:id="rId1"/>
@@ -22,17 +23,27 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'PMM SIC'!$B$1:$G$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'PMM SING'!$B$1:$G$22</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" calcMode="manual" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>fcanales</author>
   </authors>
   <commentList>
-    <comment ref="H9" authorId="0" shapeId="0">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -89,12 +100,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>fcanales</author>
   </authors>
   <commentList>
-    <comment ref="H9" authorId="0" shapeId="0">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -151,12 +162,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>fcanales</author>
   </authors>
   <commentList>
-    <comment ref="H9" authorId="0" shapeId="0">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1430,30 +1441,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="20">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-340A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000;[Red]\-#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="\$#,##0\ ;\(\$#,##0\)"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="0.0000000"/>
-    <numFmt numFmtId="181" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="16">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-340A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="\$#,##0\ ;\(\$#,##0\)"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="180" formatCode="0.0000"/>
+    <numFmt numFmtId="181" formatCode="0.0000000"/>
+    <numFmt numFmtId="182" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1527,11 +1534,6 @@
       <color indexed="22"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2033,7 +2035,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="361">
+  <cellStyleXfs count="357">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="0">
@@ -2046,11 +2048,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2115,18 +2113,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="3" fontId="15" fillId="2" borderId="2">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="14" fillId="2" borderId="2">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2259,7 +2257,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2276,72 +2274,72 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2397,20 +2395,20 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="8" fillId="5" borderId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="5" borderId="0">
+    <xf numFmtId="3" fontId="16" fillId="5" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="15" fillId="6" borderId="2">
+    <xf numFmtId="3" fontId="14" fillId="6" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="5" borderId="0">
+    <xf numFmtId="3" fontId="17" fillId="5" borderId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="7" borderId="0">
@@ -2419,588 +2417,584 @@
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="222" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="218" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="7" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="8" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="8" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="9" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="9" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="10" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="10" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="11" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="11" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="12" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="9" borderId="12" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="13" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="13" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="14" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="14" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="14" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="14" xfId="82" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="14" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="14" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="10" borderId="15" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="10" borderId="15" xfId="218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="16" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="16" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="15" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="15" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="17" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="17" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="80" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="76" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="18" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="18" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="82" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="1" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="1" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="10" borderId="19" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="10" borderId="19" xfId="218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="20" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="20" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="19" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="19" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="21" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="21" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="222" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="218" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="21" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="21" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="7" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="7" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="9" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="9" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="10" borderId="10" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="10" borderId="10" xfId="218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="11" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="11" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="10" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="10" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="12" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="12" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="22" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="22" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="23" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="23" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="23" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="23" xfId="82" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="23" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="23" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="10" borderId="24" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="10" borderId="24" xfId="218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="25" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="10" borderId="25" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="24" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="24" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="10" borderId="26" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="26" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="9" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="9" xfId="82" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="9" xfId="86" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="9" xfId="82" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="2" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="86" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="10" borderId="27" xfId="222" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="10" borderId="27" xfId="218" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="361">
-    <cellStyle name="0,0_x000a__x000a_NA_x000a__x000a_" xfId="1"/>
-    <cellStyle name="1o.nível" xfId="2"/>
-    <cellStyle name="2o.nível" xfId="3"/>
-    <cellStyle name="a_quebra_2" xfId="4"/>
-    <cellStyle name="A3 297 x 420 mm" xfId="5"/>
-    <cellStyle name="Cabecera 1" xfId="6"/>
-    <cellStyle name="Cabecera 2" xfId="7"/>
-    <cellStyle name="Comma [0]_Bce ultramundo(1)" xfId="8"/>
-    <cellStyle name="Comma_Bce ultramundo(1)" xfId="9"/>
-    <cellStyle name="Currency [0]_Bce ultramundo(1)" xfId="10"/>
-    <cellStyle name="Currency_Bce ultramundo(1)" xfId="11"/>
-    <cellStyle name="Euro" xfId="12"/>
-    <cellStyle name="Euro 10" xfId="13"/>
-    <cellStyle name="Euro 11" xfId="14"/>
-    <cellStyle name="Euro 12" xfId="15"/>
-    <cellStyle name="Euro 13" xfId="16"/>
-    <cellStyle name="Euro 14" xfId="17"/>
-    <cellStyle name="Euro 15" xfId="18"/>
-    <cellStyle name="Euro 16" xfId="19"/>
-    <cellStyle name="Euro 17" xfId="20"/>
-    <cellStyle name="Euro 18" xfId="21"/>
-    <cellStyle name="Euro 19" xfId="22"/>
-    <cellStyle name="Euro 2" xfId="23"/>
-    <cellStyle name="Euro 20" xfId="24"/>
-    <cellStyle name="Euro 21" xfId="25"/>
-    <cellStyle name="Euro 22" xfId="26"/>
-    <cellStyle name="Euro 23" xfId="27"/>
-    <cellStyle name="Euro 24" xfId="28"/>
-    <cellStyle name="Euro 25" xfId="29"/>
-    <cellStyle name="Euro 26" xfId="30"/>
-    <cellStyle name="Euro 27" xfId="31"/>
-    <cellStyle name="Euro 28" xfId="32"/>
-    <cellStyle name="Euro 29" xfId="33"/>
-    <cellStyle name="Euro 3" xfId="34"/>
-    <cellStyle name="Euro 30" xfId="35"/>
-    <cellStyle name="Euro 31" xfId="36"/>
-    <cellStyle name="Euro 32" xfId="37"/>
-    <cellStyle name="Euro 33" xfId="38"/>
-    <cellStyle name="Euro 34" xfId="39"/>
-    <cellStyle name="Euro 35" xfId="40"/>
-    <cellStyle name="Euro 36" xfId="41"/>
-    <cellStyle name="Euro 37" xfId="42"/>
-    <cellStyle name="Euro 38" xfId="43"/>
-    <cellStyle name="Euro 39" xfId="44"/>
-    <cellStyle name="Euro 4" xfId="45"/>
-    <cellStyle name="Euro 40" xfId="46"/>
-    <cellStyle name="Euro 41" xfId="47"/>
-    <cellStyle name="Euro 42" xfId="48"/>
-    <cellStyle name="Euro 43" xfId="49"/>
-    <cellStyle name="Euro 44" xfId="50"/>
-    <cellStyle name="Euro 45" xfId="51"/>
-    <cellStyle name="Euro 46" xfId="52"/>
-    <cellStyle name="Euro 47" xfId="53"/>
-    <cellStyle name="Euro 48" xfId="54"/>
-    <cellStyle name="Euro 49" xfId="55"/>
-    <cellStyle name="Euro 5" xfId="56"/>
-    <cellStyle name="Euro 50" xfId="57"/>
-    <cellStyle name="Euro 51" xfId="58"/>
-    <cellStyle name="Euro 52" xfId="59"/>
-    <cellStyle name="Euro 53" xfId="60"/>
-    <cellStyle name="Euro 54" xfId="61"/>
-    <cellStyle name="Euro 55" xfId="62"/>
-    <cellStyle name="Euro 56" xfId="63"/>
-    <cellStyle name="Euro 57" xfId="64"/>
-    <cellStyle name="Euro 58" xfId="65"/>
-    <cellStyle name="Euro 59" xfId="66"/>
-    <cellStyle name="Euro 6" xfId="67"/>
-    <cellStyle name="Euro 60" xfId="68"/>
-    <cellStyle name="Euro 61" xfId="69"/>
-    <cellStyle name="Euro 62" xfId="70"/>
-    <cellStyle name="Euro 63" xfId="71"/>
-    <cellStyle name="Euro 64" xfId="72"/>
-    <cellStyle name="Euro 7" xfId="73"/>
-    <cellStyle name="Euro 8" xfId="74"/>
-    <cellStyle name="Euro 9" xfId="75"/>
-    <cellStyle name="Euro_SIC PNLP Gx" xfId="76"/>
-    <cellStyle name="Fecha" xfId="77"/>
-    <cellStyle name="Fijo" xfId="78"/>
-    <cellStyle name="Hyperlink" xfId="79"/>
-    <cellStyle name="Millares" xfId="80" builtinId="3"/>
-    <cellStyle name="Millares 2" xfId="81"/>
-    <cellStyle name="Millares 3" xfId="82"/>
-    <cellStyle name="Millares 4" xfId="83"/>
-    <cellStyle name="Monetario0" xfId="84"/>
-    <cellStyle name="movimentação" xfId="85"/>
+  <cellStyles count="357">
+    <cellStyle name="0,0_x000a__x000a_NA_x000a__x000a_" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="1o.nível" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="2o.nível" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="a_quebra_2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="A3 297 x 420 mm" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Cabecera 1" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Cabecera 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma" xfId="76" builtinId="3"/>
+    <cellStyle name="Euro" xfId="8" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Euro 10" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Euro 11" xfId="10" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Euro 12" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Euro 13" xfId="12" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Euro 14" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Euro 15" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Euro 16" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Euro 17" xfId="16" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Euro 18" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Euro 19" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Euro 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Euro 20" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Euro 21" xfId="21" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Euro 22" xfId="22" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Euro 23" xfId="23" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Euro 24" xfId="24" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Euro 25" xfId="25" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Euro 26" xfId="26" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Euro 27" xfId="27" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Euro 28" xfId="28" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Euro 29" xfId="29" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Euro 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Euro 30" xfId="31" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Euro 31" xfId="32" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Euro 32" xfId="33" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Euro 33" xfId="34" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Euro 34" xfId="35" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Euro 35" xfId="36" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Euro 36" xfId="37" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Euro 37" xfId="38" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Euro 38" xfId="39" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Euro 39" xfId="40" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Euro 4" xfId="41" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Euro 40" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Euro 41" xfId="43" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Euro 42" xfId="44" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Euro 43" xfId="45" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Euro 44" xfId="46" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Euro 45" xfId="47" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Euro 46" xfId="48" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Euro 47" xfId="49" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Euro 48" xfId="50" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Euro 49" xfId="51" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Euro 5" xfId="52" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Euro 50" xfId="53" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Euro 51" xfId="54" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Euro 52" xfId="55" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Euro 53" xfId="56" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Euro 54" xfId="57" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Euro 55" xfId="58" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Euro 56" xfId="59" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Euro 57" xfId="60" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Euro 58" xfId="61" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Euro 59" xfId="62" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Euro 6" xfId="63" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Euro 60" xfId="64" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Euro 61" xfId="65" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Euro 62" xfId="66" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Euro 63" xfId="67" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Euro 64" xfId="68" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Euro 7" xfId="69" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Euro 8" xfId="70" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Euro 9" xfId="71" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Euro_SIC PNLP Gx" xfId="72" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Fecha" xfId="73" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Fijo" xfId="74" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Hyperlink" xfId="75" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Millares 2" xfId="77" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Millares 3" xfId="78" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Millares 4" xfId="79" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Monetario0" xfId="80" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="movimentação" xfId="81" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="86"/>
-    <cellStyle name="Normal 11" xfId="87"/>
-    <cellStyle name="Normal 12" xfId="88"/>
-    <cellStyle name="Normal 13" xfId="89"/>
-    <cellStyle name="Normal 14" xfId="90"/>
-    <cellStyle name="Normal 15" xfId="91"/>
-    <cellStyle name="Normal 16" xfId="92"/>
-    <cellStyle name="Normal 17" xfId="93"/>
-    <cellStyle name="Normal 18" xfId="94"/>
-    <cellStyle name="Normal 19" xfId="95"/>
-    <cellStyle name="Normal 2" xfId="96"/>
-    <cellStyle name="Normal 2 10" xfId="97"/>
-    <cellStyle name="Normal 2 11" xfId="98"/>
-    <cellStyle name="Normal 2 12" xfId="99"/>
-    <cellStyle name="Normal 2 13" xfId="100"/>
-    <cellStyle name="Normal 2 14" xfId="101"/>
-    <cellStyle name="Normal 2 15" xfId="102"/>
-    <cellStyle name="Normal 2 16" xfId="103"/>
-    <cellStyle name="Normal 2 17" xfId="104"/>
-    <cellStyle name="Normal 2 18" xfId="105"/>
-    <cellStyle name="Normal 2 19" xfId="106"/>
-    <cellStyle name="Normal 2 2" xfId="107"/>
-    <cellStyle name="Normal 2 20" xfId="108"/>
-    <cellStyle name="Normal 2 21" xfId="109"/>
-    <cellStyle name="Normal 2 22" xfId="110"/>
-    <cellStyle name="Normal 2 23" xfId="111"/>
-    <cellStyle name="Normal 2 24" xfId="112"/>
-    <cellStyle name="Normal 2 25" xfId="113"/>
-    <cellStyle name="Normal 2 26" xfId="114"/>
-    <cellStyle name="Normal 2 27" xfId="115"/>
-    <cellStyle name="Normal 2 28" xfId="116"/>
-    <cellStyle name="Normal 2 29" xfId="117"/>
-    <cellStyle name="Normal 2 3" xfId="118"/>
-    <cellStyle name="Normal 2 30" xfId="119"/>
-    <cellStyle name="Normal 2 31" xfId="120"/>
-    <cellStyle name="Normal 2 32" xfId="121"/>
-    <cellStyle name="Normal 2 33" xfId="122"/>
-    <cellStyle name="Normal 2 34" xfId="123"/>
-    <cellStyle name="Normal 2 35" xfId="124"/>
-    <cellStyle name="Normal 2 36" xfId="125"/>
-    <cellStyle name="Normal 2 37" xfId="126"/>
-    <cellStyle name="Normal 2 38" xfId="127"/>
-    <cellStyle name="Normal 2 39" xfId="128"/>
-    <cellStyle name="Normal 2 4" xfId="129"/>
-    <cellStyle name="Normal 2 40" xfId="130"/>
-    <cellStyle name="Normal 2 41" xfId="131"/>
-    <cellStyle name="Normal 2 42" xfId="132"/>
-    <cellStyle name="Normal 2 43" xfId="133"/>
-    <cellStyle name="Normal 2 44" xfId="134"/>
-    <cellStyle name="Normal 2 45" xfId="135"/>
-    <cellStyle name="Normal 2 46" xfId="136"/>
-    <cellStyle name="Normal 2 47" xfId="137"/>
-    <cellStyle name="Normal 2 48" xfId="138"/>
-    <cellStyle name="Normal 2 49" xfId="139"/>
-    <cellStyle name="Normal 2 5" xfId="140"/>
-    <cellStyle name="Normal 2 50" xfId="141"/>
-    <cellStyle name="Normal 2 51" xfId="142"/>
-    <cellStyle name="Normal 2 52" xfId="143"/>
-    <cellStyle name="Normal 2 53" xfId="144"/>
-    <cellStyle name="Normal 2 54" xfId="145"/>
-    <cellStyle name="Normal 2 55" xfId="146"/>
-    <cellStyle name="Normal 2 56" xfId="147"/>
-    <cellStyle name="Normal 2 57" xfId="148"/>
-    <cellStyle name="Normal 2 58" xfId="149"/>
-    <cellStyle name="Normal 2 59" xfId="150"/>
-    <cellStyle name="Normal 2 6" xfId="151"/>
-    <cellStyle name="Normal 2 60" xfId="152"/>
-    <cellStyle name="Normal 2 61" xfId="153"/>
-    <cellStyle name="Normal 2 62" xfId="154"/>
-    <cellStyle name="Normal 2 63" xfId="155"/>
-    <cellStyle name="Normal 2 64" xfId="156"/>
-    <cellStyle name="Normal 2 65" xfId="157"/>
-    <cellStyle name="Normal 2 66" xfId="158"/>
-    <cellStyle name="Normal 2 67" xfId="159"/>
-    <cellStyle name="Normal 2 7" xfId="160"/>
-    <cellStyle name="Normal 2 8" xfId="161"/>
-    <cellStyle name="Normal 2 9" xfId="162"/>
-    <cellStyle name="Normal 2_SIC PNLP Gx" xfId="163"/>
-    <cellStyle name="Normal 20" xfId="164"/>
-    <cellStyle name="Normal 21" xfId="165"/>
-    <cellStyle name="Normal 22" xfId="166"/>
-    <cellStyle name="Normal 23" xfId="167"/>
-    <cellStyle name="Normal 24" xfId="168"/>
-    <cellStyle name="Normal 25" xfId="169"/>
-    <cellStyle name="Normal 26" xfId="170"/>
-    <cellStyle name="Normal 27" xfId="171"/>
-    <cellStyle name="Normal 28" xfId="172"/>
-    <cellStyle name="Normal 29" xfId="173"/>
-    <cellStyle name="Normal 3" xfId="174"/>
-    <cellStyle name="Normal 30" xfId="175"/>
-    <cellStyle name="Normal 31" xfId="176"/>
-    <cellStyle name="Normal 32" xfId="177"/>
-    <cellStyle name="Normal 33" xfId="178"/>
-    <cellStyle name="Normal 34" xfId="179"/>
-    <cellStyle name="Normal 35" xfId="180"/>
-    <cellStyle name="Normal 36" xfId="181"/>
-    <cellStyle name="Normal 37" xfId="182"/>
-    <cellStyle name="Normal 38" xfId="183"/>
-    <cellStyle name="Normal 39" xfId="184"/>
-    <cellStyle name="Normal 4" xfId="185"/>
-    <cellStyle name="Normal 40" xfId="186"/>
-    <cellStyle name="Normal 41" xfId="187"/>
-    <cellStyle name="Normal 42" xfId="188"/>
-    <cellStyle name="Normal 43" xfId="189"/>
-    <cellStyle name="Normal 44" xfId="190"/>
-    <cellStyle name="Normal 45" xfId="191"/>
-    <cellStyle name="Normal 46" xfId="192"/>
-    <cellStyle name="Normal 47" xfId="193"/>
-    <cellStyle name="Normal 48" xfId="194"/>
-    <cellStyle name="Normal 49" xfId="195"/>
-    <cellStyle name="Normal 5" xfId="196"/>
-    <cellStyle name="Normal 50" xfId="197"/>
-    <cellStyle name="Normal 51" xfId="198"/>
-    <cellStyle name="Normal 52" xfId="199"/>
-    <cellStyle name="Normal 53" xfId="200"/>
-    <cellStyle name="Normal 54" xfId="201"/>
-    <cellStyle name="Normal 55" xfId="202"/>
-    <cellStyle name="Normal 56" xfId="203"/>
-    <cellStyle name="Normal 57" xfId="204"/>
-    <cellStyle name="Normal 58" xfId="205"/>
-    <cellStyle name="Normal 59" xfId="206"/>
-    <cellStyle name="Normal 6" xfId="207"/>
-    <cellStyle name="Normal 60" xfId="208"/>
-    <cellStyle name="Normal 61" xfId="209"/>
-    <cellStyle name="Normal 62" xfId="210"/>
-    <cellStyle name="Normal 63" xfId="211"/>
-    <cellStyle name="Normal 64" xfId="212"/>
-    <cellStyle name="Normal 65" xfId="213"/>
-    <cellStyle name="Normal 66" xfId="214"/>
-    <cellStyle name="Normal 67" xfId="215"/>
-    <cellStyle name="Normal 68" xfId="216"/>
-    <cellStyle name="Normal 7" xfId="217"/>
-    <cellStyle name="Normal 8" xfId="218"/>
-    <cellStyle name="Normal 9" xfId="219"/>
-    <cellStyle name="Notas 2" xfId="220"/>
-    <cellStyle name="Notas 3" xfId="221"/>
-    <cellStyle name="Porcentual 10" xfId="222"/>
-    <cellStyle name="Porcentual 11" xfId="223"/>
-    <cellStyle name="Porcentual 12" xfId="224"/>
-    <cellStyle name="Porcentual 13" xfId="225"/>
-    <cellStyle name="Porcentual 14" xfId="226"/>
-    <cellStyle name="Porcentual 15" xfId="227"/>
-    <cellStyle name="Porcentual 16" xfId="228"/>
-    <cellStyle name="Porcentual 17" xfId="229"/>
-    <cellStyle name="Porcentual 18" xfId="230"/>
-    <cellStyle name="Porcentual 19" xfId="231"/>
-    <cellStyle name="Porcentual 2" xfId="232"/>
-    <cellStyle name="Porcentual 2 10" xfId="233"/>
-    <cellStyle name="Porcentual 2 11" xfId="234"/>
-    <cellStyle name="Porcentual 2 12" xfId="235"/>
-    <cellStyle name="Porcentual 2 13" xfId="236"/>
-    <cellStyle name="Porcentual 2 14" xfId="237"/>
-    <cellStyle name="Porcentual 2 15" xfId="238"/>
-    <cellStyle name="Porcentual 2 16" xfId="239"/>
-    <cellStyle name="Porcentual 2 17" xfId="240"/>
-    <cellStyle name="Porcentual 2 18" xfId="241"/>
-    <cellStyle name="Porcentual 2 19" xfId="242"/>
-    <cellStyle name="Porcentual 2 2" xfId="243"/>
-    <cellStyle name="Porcentual 2 20" xfId="244"/>
-    <cellStyle name="Porcentual 2 21" xfId="245"/>
-    <cellStyle name="Porcentual 2 22" xfId="246"/>
-    <cellStyle name="Porcentual 2 23" xfId="247"/>
-    <cellStyle name="Porcentual 2 24" xfId="248"/>
-    <cellStyle name="Porcentual 2 25" xfId="249"/>
-    <cellStyle name="Porcentual 2 26" xfId="250"/>
-    <cellStyle name="Porcentual 2 27" xfId="251"/>
-    <cellStyle name="Porcentual 2 28" xfId="252"/>
-    <cellStyle name="Porcentual 2 29" xfId="253"/>
-    <cellStyle name="Porcentual 2 3" xfId="254"/>
-    <cellStyle name="Porcentual 2 30" xfId="255"/>
-    <cellStyle name="Porcentual 2 31" xfId="256"/>
-    <cellStyle name="Porcentual 2 32" xfId="257"/>
-    <cellStyle name="Porcentual 2 33" xfId="258"/>
-    <cellStyle name="Porcentual 2 34" xfId="259"/>
-    <cellStyle name="Porcentual 2 35" xfId="260"/>
-    <cellStyle name="Porcentual 2 36" xfId="261"/>
-    <cellStyle name="Porcentual 2 37" xfId="262"/>
-    <cellStyle name="Porcentual 2 38" xfId="263"/>
-    <cellStyle name="Porcentual 2 39" xfId="264"/>
-    <cellStyle name="Porcentual 2 4" xfId="265"/>
-    <cellStyle name="Porcentual 2 40" xfId="266"/>
-    <cellStyle name="Porcentual 2 41" xfId="267"/>
-    <cellStyle name="Porcentual 2 42" xfId="268"/>
-    <cellStyle name="Porcentual 2 43" xfId="269"/>
-    <cellStyle name="Porcentual 2 44" xfId="270"/>
-    <cellStyle name="Porcentual 2 45" xfId="271"/>
-    <cellStyle name="Porcentual 2 46" xfId="272"/>
-    <cellStyle name="Porcentual 2 47" xfId="273"/>
-    <cellStyle name="Porcentual 2 48" xfId="274"/>
-    <cellStyle name="Porcentual 2 49" xfId="275"/>
-    <cellStyle name="Porcentual 2 5" xfId="276"/>
-    <cellStyle name="Porcentual 2 50" xfId="277"/>
-    <cellStyle name="Porcentual 2 51" xfId="278"/>
-    <cellStyle name="Porcentual 2 52" xfId="279"/>
-    <cellStyle name="Porcentual 2 53" xfId="280"/>
-    <cellStyle name="Porcentual 2 54" xfId="281"/>
-    <cellStyle name="Porcentual 2 55" xfId="282"/>
-    <cellStyle name="Porcentual 2 56" xfId="283"/>
-    <cellStyle name="Porcentual 2 57" xfId="284"/>
-    <cellStyle name="Porcentual 2 58" xfId="285"/>
-    <cellStyle name="Porcentual 2 59" xfId="286"/>
-    <cellStyle name="Porcentual 2 6" xfId="287"/>
-    <cellStyle name="Porcentual 2 60" xfId="288"/>
-    <cellStyle name="Porcentual 2 61" xfId="289"/>
-    <cellStyle name="Porcentual 2 62" xfId="290"/>
-    <cellStyle name="Porcentual 2 63" xfId="291"/>
-    <cellStyle name="Porcentual 2 64" xfId="292"/>
-    <cellStyle name="Porcentual 2 65" xfId="293"/>
-    <cellStyle name="Porcentual 2 66" xfId="294"/>
-    <cellStyle name="Porcentual 2 67" xfId="295"/>
-    <cellStyle name="Porcentual 2 7" xfId="296"/>
-    <cellStyle name="Porcentual 2 8" xfId="297"/>
-    <cellStyle name="Porcentual 2 9" xfId="298"/>
-    <cellStyle name="Porcentual 20" xfId="299"/>
-    <cellStyle name="Porcentual 21" xfId="300"/>
-    <cellStyle name="Porcentual 22" xfId="301"/>
-    <cellStyle name="Porcentual 23" xfId="302"/>
-    <cellStyle name="Porcentual 24" xfId="303"/>
-    <cellStyle name="Porcentual 25" xfId="304"/>
-    <cellStyle name="Porcentual 26" xfId="305"/>
-    <cellStyle name="Porcentual 27" xfId="306"/>
-    <cellStyle name="Porcentual 28" xfId="307"/>
-    <cellStyle name="Porcentual 29" xfId="308"/>
-    <cellStyle name="Porcentual 3" xfId="309"/>
-    <cellStyle name="Porcentual 30" xfId="310"/>
-    <cellStyle name="Porcentual 31" xfId="311"/>
-    <cellStyle name="Porcentual 32" xfId="312"/>
-    <cellStyle name="Porcentual 33" xfId="313"/>
-    <cellStyle name="Porcentual 34" xfId="314"/>
-    <cellStyle name="Porcentual 35" xfId="315"/>
-    <cellStyle name="Porcentual 36" xfId="316"/>
-    <cellStyle name="Porcentual 37" xfId="317"/>
-    <cellStyle name="Porcentual 38" xfId="318"/>
-    <cellStyle name="Porcentual 39" xfId="319"/>
-    <cellStyle name="Porcentual 4" xfId="320"/>
-    <cellStyle name="Porcentual 40" xfId="321"/>
-    <cellStyle name="Porcentual 41" xfId="322"/>
-    <cellStyle name="Porcentual 42" xfId="323"/>
-    <cellStyle name="Porcentual 43" xfId="324"/>
-    <cellStyle name="Porcentual 44" xfId="325"/>
-    <cellStyle name="Porcentual 45" xfId="326"/>
-    <cellStyle name="Porcentual 46" xfId="327"/>
-    <cellStyle name="Porcentual 47" xfId="328"/>
-    <cellStyle name="Porcentual 48" xfId="329"/>
-    <cellStyle name="Porcentual 49" xfId="330"/>
-    <cellStyle name="Porcentual 5" xfId="331"/>
-    <cellStyle name="Porcentual 50" xfId="332"/>
-    <cellStyle name="Porcentual 51" xfId="333"/>
-    <cellStyle name="Porcentual 52" xfId="334"/>
-    <cellStyle name="Porcentual 53" xfId="335"/>
-    <cellStyle name="Porcentual 54" xfId="336"/>
-    <cellStyle name="Porcentual 55" xfId="337"/>
-    <cellStyle name="Porcentual 56" xfId="338"/>
-    <cellStyle name="Porcentual 57" xfId="339"/>
-    <cellStyle name="Porcentual 58" xfId="340"/>
-    <cellStyle name="Porcentual 59" xfId="341"/>
-    <cellStyle name="Porcentual 6" xfId="342"/>
-    <cellStyle name="Porcentual 60" xfId="343"/>
-    <cellStyle name="Porcentual 61" xfId="344"/>
-    <cellStyle name="Porcentual 62" xfId="345"/>
-    <cellStyle name="Porcentual 63" xfId="346"/>
-    <cellStyle name="Porcentual 64" xfId="347"/>
-    <cellStyle name="Porcentual 65" xfId="348"/>
-    <cellStyle name="Porcentual 66" xfId="349"/>
-    <cellStyle name="Porcentual 67" xfId="350"/>
-    <cellStyle name="Porcentual 7" xfId="351"/>
-    <cellStyle name="Porcentual 8" xfId="352"/>
-    <cellStyle name="Porcentual 9" xfId="353"/>
-    <cellStyle name="Punto0" xfId="354"/>
-    <cellStyle name="ssubtitulo" xfId="355"/>
-    <cellStyle name="subtitulo" xfId="356"/>
-    <cellStyle name="titulo" xfId="357"/>
-    <cellStyle name="titulomov" xfId="358"/>
-    <cellStyle name="Todos" xfId="359"/>
-    <cellStyle name="totalbalan" xfId="360"/>
+    <cellStyle name="Normal 10" xfId="82" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 11" xfId="83" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 12" xfId="84" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 13" xfId="85" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 14" xfId="86" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 15" xfId="87" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 16" xfId="88" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 17" xfId="89" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 18" xfId="90" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 19" xfId="91" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 2 10" xfId="93" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 2 11" xfId="94" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 2 12" xfId="95" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 2 13" xfId="96" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 2 14" xfId="97" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 2 15" xfId="98" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 2 16" xfId="99" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 2 17" xfId="100" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 2 18" xfId="101" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 2 19" xfId="102" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 2 2" xfId="103" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 2 20" xfId="104" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 2 21" xfId="105" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 2 22" xfId="106" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 2 23" xfId="107" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 2 24" xfId="108" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 2 25" xfId="109" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 2 26" xfId="110" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 2 27" xfId="111" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 2 28" xfId="112" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 2 29" xfId="113" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 2 3" xfId="114" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 2 30" xfId="115" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 2 31" xfId="116" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 2 32" xfId="117" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 2 33" xfId="118" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 2 34" xfId="119" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 2 35" xfId="120" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 2 36" xfId="121" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 2 37" xfId="122" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 2 38" xfId="123" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 2 39" xfId="124" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 2 4" xfId="125" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 2 40" xfId="126" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 2 41" xfId="127" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 2 42" xfId="128" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 2 43" xfId="129" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 2 44" xfId="130" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 2 45" xfId="131" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 2 46" xfId="132" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 2 47" xfId="133" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 2 48" xfId="134" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 2 49" xfId="135" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 2 5" xfId="136" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 2 50" xfId="137" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 2 51" xfId="138" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 2 52" xfId="139" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 2 53" xfId="140" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 2 54" xfId="141" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 2 55" xfId="142" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 2 56" xfId="143" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 2 57" xfId="144" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 2 58" xfId="145" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 2 59" xfId="146" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 2 60" xfId="148" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 2 61" xfId="149" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 2 62" xfId="150" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 2 63" xfId="151" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 2 64" xfId="152" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 2 65" xfId="153" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 2 66" xfId="154" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 2 67" xfId="155" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 2 7" xfId="156" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 2 8" xfId="157" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 2 9" xfId="158" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 2_SIC PNLP Gx" xfId="159" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 20" xfId="160" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 21" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 22" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 23" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 24" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 25" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 26" xfId="166" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 27" xfId="167" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 28" xfId="168" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 29" xfId="169" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 3" xfId="170" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 30" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Normal 31" xfId="172" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Normal 32" xfId="173" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Normal 33" xfId="174" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Normal 34" xfId="175" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Normal 35" xfId="176" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Normal 36" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Normal 37" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Normal 38" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Normal 39" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Normal 4" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Normal 40" xfId="182" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Normal 41" xfId="183" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Normal 42" xfId="184" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Normal 43" xfId="185" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Normal 44" xfId="186" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Normal 45" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Normal 46" xfId="188" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Normal 47" xfId="189" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Normal 48" xfId="190" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Normal 49" xfId="191" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Normal 5" xfId="192" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Normal 50" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Normal 51" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Normal 52" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Normal 53" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Normal 54" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Normal 55" xfId="198" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Normal 56" xfId="199" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Normal 57" xfId="200" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Normal 58" xfId="201" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Normal 59" xfId="202" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Normal 6" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Normal 60" xfId="204" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Normal 61" xfId="205" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Normal 62" xfId="206" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Normal 63" xfId="207" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Normal 64" xfId="208" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Normal 65" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Normal 66" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Normal 67" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Normal 68" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Normal 7" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Normal 8" xfId="214" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Normal 9" xfId="215" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Notas 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Notas 3" xfId="217" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Porcentual 10" xfId="218" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Porcentual 11" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Porcentual 12" xfId="220" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Porcentual 13" xfId="221" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Porcentual 14" xfId="222" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Porcentual 15" xfId="223" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Porcentual 16" xfId="224" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Porcentual 17" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Porcentual 18" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Porcentual 19" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Porcentual 2" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Porcentual 2 10" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Porcentual 2 11" xfId="230" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Porcentual 2 12" xfId="231" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Porcentual 2 13" xfId="232" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Porcentual 2 14" xfId="233" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Porcentual 2 15" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Porcentual 2 16" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Porcentual 2 17" xfId="236" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Porcentual 2 18" xfId="237" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Porcentual 2 19" xfId="238" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Porcentual 2 2" xfId="239" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Porcentual 2 20" xfId="240" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Porcentual 2 21" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Porcentual 2 22" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Porcentual 2 23" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Porcentual 2 24" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Porcentual 2 25" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Porcentual 2 26" xfId="246" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Porcentual 2 27" xfId="247" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Porcentual 2 28" xfId="248" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Porcentual 2 29" xfId="249" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Porcentual 2 3" xfId="250" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Porcentual 2 30" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Porcentual 2 31" xfId="252" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Porcentual 2 32" xfId="253" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Porcentual 2 33" xfId="254" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Porcentual 2 34" xfId="255" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Porcentual 2 35" xfId="256" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Porcentual 2 36" xfId="257" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Porcentual 2 37" xfId="258" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Porcentual 2 38" xfId="259" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Porcentual 2 39" xfId="260" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Porcentual 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Porcentual 2 40" xfId="262" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Porcentual 2 41" xfId="263" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Porcentual 2 42" xfId="264" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Porcentual 2 43" xfId="265" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Porcentual 2 44" xfId="266" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Porcentual 2 45" xfId="267" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Porcentual 2 46" xfId="268" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Porcentual 2 47" xfId="269" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Porcentual 2 48" xfId="270" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Porcentual 2 49" xfId="271" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Porcentual 2 5" xfId="272" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Porcentual 2 50" xfId="273" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Porcentual 2 51" xfId="274" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Porcentual 2 52" xfId="275" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Porcentual 2 53" xfId="276" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Porcentual 2 54" xfId="277" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Porcentual 2 55" xfId="278" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Porcentual 2 56" xfId="279" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Porcentual 2 57" xfId="280" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Porcentual 2 58" xfId="281" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Porcentual 2 59" xfId="282" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Porcentual 2 6" xfId="283" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Porcentual 2 60" xfId="284" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Porcentual 2 61" xfId="285" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Porcentual 2 62" xfId="286" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Porcentual 2 63" xfId="287" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Porcentual 2 64" xfId="288" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Porcentual 2 65" xfId="289" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Porcentual 2 66" xfId="290" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Porcentual 2 67" xfId="291" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Porcentual 2 7" xfId="292" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Porcentual 2 8" xfId="293" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Porcentual 2 9" xfId="294" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Porcentual 20" xfId="295" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Porcentual 21" xfId="296" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Porcentual 22" xfId="297" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Porcentual 23" xfId="298" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Porcentual 24" xfId="299" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Porcentual 25" xfId="300" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Porcentual 26" xfId="301" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Porcentual 27" xfId="302" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Porcentual 28" xfId="303" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Porcentual 29" xfId="304" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Porcentual 3" xfId="305" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Porcentual 30" xfId="306" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Porcentual 31" xfId="307" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Porcentual 32" xfId="308" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Porcentual 33" xfId="309" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Porcentual 34" xfId="310" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Porcentual 35" xfId="311" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Porcentual 36" xfId="312" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Porcentual 37" xfId="313" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Porcentual 38" xfId="314" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Porcentual 39" xfId="315" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Porcentual 4" xfId="316" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Porcentual 40" xfId="317" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Porcentual 41" xfId="318" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Porcentual 42" xfId="319" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Porcentual 43" xfId="320" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Porcentual 44" xfId="321" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Porcentual 45" xfId="322" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Porcentual 46" xfId="323" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Porcentual 47" xfId="324" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Porcentual 48" xfId="325" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Porcentual 49" xfId="326" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Porcentual 5" xfId="327" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Porcentual 50" xfId="328" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Porcentual 51" xfId="329" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Porcentual 52" xfId="330" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Porcentual 53" xfId="331" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Porcentual 54" xfId="332" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Porcentual 55" xfId="333" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Porcentual 56" xfId="334" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Porcentual 57" xfId="335" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Porcentual 58" xfId="336" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Porcentual 59" xfId="337" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Porcentual 6" xfId="338" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Porcentual 60" xfId="339" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Porcentual 61" xfId="340" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Porcentual 62" xfId="341" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Porcentual 63" xfId="342" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Porcentual 64" xfId="343" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Porcentual 65" xfId="344" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Porcentual 66" xfId="345" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Porcentual 67" xfId="346" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Porcentual 7" xfId="347" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Porcentual 8" xfId="348" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Porcentual 9" xfId="349" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Punto0" xfId="350" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="ssubtitulo" xfId="351" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="subtitulo" xfId="352" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="titulo" xfId="353" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="titulomov" xfId="354" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Todos" xfId="355" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="totalbalan" xfId="356" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3032,7 +3026,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3184" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg"/>
+        <xdr:cNvPr id="3184" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000700C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3105,7 +3105,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1304" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg"/>
+        <xdr:cNvPr id="1304" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018050000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3178,7 +3184,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2159" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg"/>
+        <xdr:cNvPr id="2159" name="2 Imagen" descr="Logo_Comisión_Nacional_de_Energía (2).jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00006F080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3235,7 +3247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3310,6 +3322,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3345,6 +3374,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3520,7 +3566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3533,21 +3579,21 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3" style="6" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="6" customWidth="1"/>
-    <col min="5" max="11" width="16.5703125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="34.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" style="6" customWidth="1"/>
+    <col min="5" max="11" width="16.5" style="6" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="C4" s="2" t="s">
         <v>308</v>
       </c>
@@ -3560,12 +3606,12 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="17" thickBot="1"/>
+    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1">
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3577,7 +3623,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:14" s="5" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" s="5" customFormat="1" ht="52" thickBot="1">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
@@ -3611,7 +3657,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="B10" s="46" t="s">
         <v>301</v>
       </c>
@@ -3647,7 +3693,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="60"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14">
       <c r="B11" s="46" t="s">
         <v>321</v>
       </c>
@@ -3683,7 +3729,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="60"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" s="46" t="s">
         <v>327</v>
       </c>
@@ -3719,7 +3765,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="60"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" s="46" t="s">
         <v>328</v>
       </c>
@@ -3755,7 +3801,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="60"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" s="46" t="s">
         <v>330</v>
       </c>
@@ -3792,7 +3838,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="60"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" s="46" t="s">
         <v>339</v>
       </c>
@@ -3827,7 +3873,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="60"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" s="46" t="s">
         <v>335</v>
       </c>
@@ -3864,7 +3910,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="60"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="46" t="s">
         <v>337</v>
       </c>
@@ -3899,7 +3945,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="60"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="46" t="s">
         <v>341</v>
       </c>
@@ -3934,7 +3980,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="60"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="B19" s="46" t="s">
         <v>344</v>
       </c>
@@ -3969,7 +4015,7 @@
       <c r="L19" s="6"/>
       <c r="M19" s="60"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="46" t="s">
         <v>346</v>
       </c>
@@ -4004,7 +4050,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="60"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="46" t="s">
         <v>348</v>
       </c>
@@ -4039,7 +4085,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="60"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="46" t="s">
         <v>350</v>
       </c>
@@ -4074,7 +4120,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="60"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="46" t="s">
         <v>353</v>
       </c>
@@ -4109,7 +4155,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="60"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="46" t="s">
         <v>352</v>
       </c>
@@ -4144,7 +4190,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="60"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="46" t="s">
         <v>357</v>
       </c>
@@ -4179,7 +4225,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="60"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="46" t="s">
         <v>360</v>
       </c>
@@ -4214,7 +4260,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="60"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="46" t="s">
         <v>362</v>
       </c>
@@ -4249,7 +4295,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="60"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="46" t="s">
         <v>366</v>
       </c>
@@ -4284,7 +4330,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="60"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="46" t="s">
         <v>367</v>
       </c>
@@ -4319,7 +4365,7 @@
       <c r="L29" s="59"/>
       <c r="M29" s="26"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="46" t="s">
         <v>370</v>
       </c>
@@ -4336,7 +4382,7 @@
         <v>68.649000000000001</v>
       </c>
       <c r="G30" s="50">
-        <f>+F30/E30-1</f>
+        <f t="shared" ref="G30:G35" si="2">+F30/E30-1</f>
         <v>4.9871536061662614E-2</v>
       </c>
       <c r="H30" s="51">
@@ -4354,7 +4400,7 @@
       <c r="L30" s="59"/>
       <c r="M30" s="26"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="46" t="s">
         <v>371</v>
       </c>
@@ -4371,7 +4417,7 @@
         <v>68.319999999999993</v>
       </c>
       <c r="G31" s="50">
-        <f>+F31/E31-1</f>
+        <f t="shared" si="2"/>
         <v>4.4840031810117864E-2</v>
       </c>
       <c r="H31" s="51">
@@ -4389,7 +4435,7 @@
       <c r="L31" s="59"/>
       <c r="M31" s="26"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="46" t="s">
         <v>373</v>
       </c>
@@ -4406,7 +4452,7 @@
         <v>67.731999999999999</v>
       </c>
       <c r="G32" s="50">
-        <f>+F32/E32-1</f>
+        <f t="shared" si="2"/>
         <v>-2.9516276937184838E-2</v>
       </c>
       <c r="H32" s="51">
@@ -4424,7 +4470,7 @@
       <c r="L32" s="59"/>
       <c r="M32" s="26"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13">
       <c r="B33" s="46" t="s">
         <v>375</v>
       </c>
@@ -4441,7 +4487,7 @@
         <v>67.864999999999995</v>
       </c>
       <c r="G33" s="50">
-        <f>+F33/E33-1</f>
+        <f t="shared" si="2"/>
         <v>-2.7610614397065691E-2</v>
       </c>
       <c r="H33" s="51">
@@ -4459,7 +4505,7 @@
       <c r="L33" s="59"/>
       <c r="M33" s="26"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13">
       <c r="B34" s="46" t="s">
         <v>378</v>
       </c>
@@ -4476,7 +4522,7 @@
         <v>68.641000000000005</v>
       </c>
       <c r="G34" s="50">
-        <f>+F34/E34-1</f>
+        <f t="shared" si="2"/>
         <v>-1.6491861531407581E-2</v>
       </c>
       <c r="H34" s="51">
@@ -4494,7 +4540,7 @@
       <c r="L34" s="59"/>
       <c r="M34" s="26"/>
     </row>
-    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="17" thickBot="1">
       <c r="B35" s="38" t="s">
         <v>380</v>
       </c>
@@ -4511,7 +4557,7 @@
         <v>68.784000000000006</v>
       </c>
       <c r="G35" s="73">
-        <f>+F35/E35-1</f>
+        <f t="shared" si="2"/>
         <v>-1.4442916093534985E-2</v>
       </c>
       <c r="H35" s="41">
@@ -4529,7 +4575,7 @@
       <c r="L35" s="59"/>
       <c r="M35" s="26"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13">
       <c r="F36" s="58"/>
       <c r="G36" s="26"/>
       <c r="H36" s="58"/>
@@ -4537,7 +4583,7 @@
       <c r="J36" s="64"/>
       <c r="K36" s="64"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13">
       <c r="B37" s="1" t="s">
         <v>170</v>
       </c>
@@ -4549,14 +4595,14 @@
       <c r="J37" s="58"/>
       <c r="K37" s="58"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13">
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
       <c r="I38" s="69"/>
       <c r="J38" s="58"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13">
       <c r="B39" s="6"/>
       <c r="F39" s="58"/>
       <c r="G39" s="58"/>
@@ -4564,7 +4610,7 @@
       <c r="I39" s="69"/>
       <c r="J39" s="58"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13">
       <c r="B40" s="6"/>
       <c r="F40" s="58"/>
       <c r="G40" s="58"/>
@@ -4572,85 +4618,85 @@
       <c r="I40" s="55"/>
       <c r="K40" s="60"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13">
       <c r="F41" s="58"/>
       <c r="G41" s="58"/>
       <c r="H41" s="58"/>
       <c r="I41" s="69"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13">
       <c r="F42" s="58"/>
       <c r="G42" s="58"/>
       <c r="H42" s="64"/>
       <c r="I42" s="69"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13">
       <c r="F43" s="58"/>
       <c r="G43" s="58"/>
       <c r="H43" s="57"/>
       <c r="I43" s="69"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13">
       <c r="G44" s="58"/>
       <c r="H44" s="64"/>
       <c r="I44" s="69"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13">
       <c r="G45" s="58"/>
       <c r="H45" s="64"/>
       <c r="I45" s="69"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13">
       <c r="G46" s="58"/>
       <c r="H46" s="64"/>
       <c r="I46" s="69"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13">
       <c r="G47" s="58"/>
       <c r="H47" s="64"/>
       <c r="I47" s="69"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13">
       <c r="G48" s="58"/>
       <c r="H48" s="64"/>
       <c r="I48" s="69"/>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:9">
       <c r="G49" s="58"/>
       <c r="H49" s="64"/>
       <c r="I49" s="69"/>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:9">
       <c r="G50" s="58"/>
       <c r="H50" s="64"/>
       <c r="I50" s="69"/>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:9">
       <c r="G51" s="58"/>
       <c r="H51" s="64"/>
       <c r="I51" s="69"/>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:9">
       <c r="G52" s="58"/>
       <c r="H52" s="64"/>
       <c r="I52" s="69"/>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:9">
       <c r="G53" s="58"/>
       <c r="H53" s="64"/>
       <c r="I53" s="69"/>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:9">
       <c r="G54" s="58"/>
       <c r="H54" s="64"/>
       <c r="I54" s="69"/>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:9">
       <c r="G55" s="58"/>
       <c r="H55" s="64"/>
       <c r="I55" s="69"/>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:9">
       <c r="G56" s="58"/>
       <c r="H56" s="64"/>
       <c r="I56" s="69"/>
@@ -4664,7 +4710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4675,26 +4721,26 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2" style="6" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="6" customWidth="1"/>
-    <col min="5" max="6" width="19.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="34.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="19.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="C4" s="2" t="s">
         <v>315</v>
       </c>
@@ -4707,12 +4753,12 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="17" thickBot="1"/>
+    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1">
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -4724,7 +4770,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:14" s="5" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" s="5" customFormat="1" ht="52" thickBot="1">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
@@ -4758,7 +4804,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" s="5" customFormat="1">
       <c r="B10" s="17" t="s">
         <v>4</v>
       </c>
@@ -4790,7 +4836,7 @@
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" s="5" customFormat="1">
       <c r="B11" s="27" t="s">
         <v>7</v>
       </c>
@@ -4821,7 +4867,7 @@
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" s="5" customFormat="1">
       <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
@@ -4852,7 +4898,7 @@
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" s="5" customFormat="1">
       <c r="B13" s="27" t="s">
         <v>11</v>
       </c>
@@ -4883,7 +4929,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" s="5" customFormat="1">
       <c r="B14" s="27" t="s">
         <v>13</v>
       </c>
@@ -4914,7 +4960,7 @@
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" s="5" customFormat="1">
       <c r="B15" s="27" t="s">
         <v>15</v>
       </c>
@@ -4945,7 +4991,7 @@
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" s="5" customFormat="1">
       <c r="B16" s="27" t="s">
         <v>17</v>
       </c>
@@ -4976,7 +5022,7 @@
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" s="5" customFormat="1">
       <c r="B17" s="27" t="s">
         <v>20</v>
       </c>
@@ -5007,7 +5053,7 @@
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" s="5" customFormat="1">
       <c r="B18" s="27" t="s">
         <v>22</v>
       </c>
@@ -5038,7 +5084,7 @@
       <c r="M18" s="26"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" s="5" customFormat="1">
       <c r="B19" s="27" t="s">
         <v>24</v>
       </c>
@@ -5069,7 +5115,7 @@
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
     </row>
-    <row r="20" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" s="5" customFormat="1">
       <c r="B20" s="27" t="s">
         <v>27</v>
       </c>
@@ -5100,7 +5146,7 @@
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
     </row>
-    <row r="21" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" s="5" customFormat="1">
       <c r="B21" s="27" t="s">
         <v>29</v>
       </c>
@@ -5131,7 +5177,7 @@
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
     </row>
-    <row r="22" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" s="5" customFormat="1">
       <c r="B22" s="27" t="s">
         <v>32</v>
       </c>
@@ -5162,7 +5208,7 @@
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
     </row>
-    <row r="23" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" s="5" customFormat="1">
       <c r="B23" s="27" t="s">
         <v>35</v>
       </c>
@@ -5193,7 +5239,7 @@
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
     </row>
-    <row r="24" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" s="5" customFormat="1">
       <c r="B24" s="27" t="s">
         <v>37</v>
       </c>
@@ -5224,7 +5270,7 @@
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
     </row>
-    <row r="25" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" s="5" customFormat="1">
       <c r="B25" s="27" t="s">
         <v>39</v>
       </c>
@@ -5255,7 +5301,7 @@
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
     </row>
-    <row r="26" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" s="5" customFormat="1">
       <c r="B26" s="27" t="s">
         <v>41</v>
       </c>
@@ -5286,7 +5332,7 @@
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
     </row>
-    <row r="27" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" s="5" customFormat="1">
       <c r="B27" s="27" t="s">
         <v>43</v>
       </c>
@@ -5317,7 +5363,7 @@
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
     </row>
-    <row r="28" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" s="5" customFormat="1">
       <c r="B28" s="27" t="s">
         <v>45</v>
       </c>
@@ -5348,7 +5394,7 @@
       <c r="M28" s="26"/>
       <c r="N28" s="26"/>
     </row>
-    <row r="29" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" s="5" customFormat="1">
       <c r="B29" s="27" t="s">
         <v>48</v>
       </c>
@@ -5379,7 +5425,7 @@
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
     </row>
-    <row r="30" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" s="5" customFormat="1">
       <c r="B30" s="27" t="s">
         <v>50</v>
       </c>
@@ -5410,7 +5456,7 @@
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
     </row>
-    <row r="31" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" s="5" customFormat="1">
       <c r="B31" s="27" t="s">
         <v>52</v>
       </c>
@@ -5441,7 +5487,7 @@
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
     </row>
-    <row r="32" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" s="5" customFormat="1">
       <c r="B32" s="27" t="s">
         <v>54</v>
       </c>
@@ -5472,7 +5518,7 @@
       <c r="M32" s="26"/>
       <c r="N32" s="26"/>
     </row>
-    <row r="33" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" s="5" customFormat="1">
       <c r="B33" s="27" t="s">
         <v>57</v>
       </c>
@@ -5503,7 +5549,7 @@
       <c r="M33" s="26"/>
       <c r="N33" s="26"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15">
       <c r="B34" s="27" t="s">
         <v>59</v>
       </c>
@@ -5535,7 +5581,7 @@
       <c r="N34" s="26"/>
       <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15">
       <c r="B35" s="27" t="s">
         <v>62</v>
       </c>
@@ -5567,7 +5613,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15">
       <c r="B36" s="27" t="s">
         <v>65</v>
       </c>
@@ -5599,7 +5645,7 @@
       <c r="N36" s="26"/>
       <c r="O36" s="26"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15">
       <c r="B37" s="27" t="s">
         <v>67</v>
       </c>
@@ -5631,7 +5677,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="26"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15">
       <c r="B38" s="27" t="s">
         <v>69</v>
       </c>
@@ -5663,7 +5709,7 @@
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15">
       <c r="B39" s="27" t="s">
         <v>71</v>
       </c>
@@ -5695,7 +5741,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15">
       <c r="B40" s="27" t="s">
         <v>73</v>
       </c>
@@ -5727,7 +5773,7 @@
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15">
       <c r="B41" s="27" t="s">
         <v>76</v>
       </c>
@@ -5759,7 +5805,7 @@
       <c r="N41" s="26"/>
       <c r="O41" s="26"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15">
       <c r="B42" s="27" t="s">
         <v>78</v>
       </c>
@@ -5791,7 +5837,7 @@
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15">
       <c r="B43" s="27" t="s">
         <v>80</v>
       </c>
@@ -5823,7 +5869,7 @@
       <c r="N43" s="26"/>
       <c r="O43" s="26"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15">
       <c r="B44" s="27" t="s">
         <v>82</v>
       </c>
@@ -5855,7 +5901,7 @@
       <c r="N44" s="26"/>
       <c r="O44" s="26"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15">
       <c r="B45" s="27" t="s">
         <v>84</v>
       </c>
@@ -5887,7 +5933,7 @@
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15">
       <c r="B46" s="27" t="s">
         <v>86</v>
       </c>
@@ -5919,7 +5965,7 @@
       <c r="N46" s="26"/>
       <c r="O46" s="26"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15">
       <c r="B47" s="27" t="s">
         <v>89</v>
       </c>
@@ -5951,7 +5997,7 @@
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15">
       <c r="B48" s="27" t="s">
         <v>91</v>
       </c>
@@ -5983,7 +6029,7 @@
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15">
       <c r="B49" s="27" t="s">
         <v>93</v>
       </c>
@@ -6015,7 +6061,7 @@
       <c r="N49" s="26"/>
       <c r="O49" s="26"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15">
       <c r="B50" s="27" t="s">
         <v>95</v>
       </c>
@@ -6047,7 +6093,7 @@
       <c r="N50" s="26"/>
       <c r="O50" s="26"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15">
       <c r="B51" s="27" t="s">
         <v>97</v>
       </c>
@@ -6083,7 +6129,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="26"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15">
       <c r="B52" s="27" t="s">
         <v>100</v>
       </c>
@@ -6119,7 +6165,7 @@
       <c r="N52" s="26"/>
       <c r="O52" s="26"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15">
       <c r="B53" s="27" t="s">
         <v>103</v>
       </c>
@@ -6155,7 +6201,7 @@
       <c r="N53" s="26"/>
       <c r="O53" s="26"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15">
       <c r="B54" s="27" t="s">
         <v>105</v>
       </c>
@@ -6191,7 +6237,7 @@
       <c r="N54" s="36"/>
       <c r="O54" s="26"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15">
       <c r="B55" s="27" t="s">
         <v>107</v>
       </c>
@@ -6227,7 +6273,7 @@
       <c r="N55" s="36"/>
       <c r="O55" s="26"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15">
       <c r="B56" s="27" t="s">
         <v>109</v>
       </c>
@@ -6263,7 +6309,7 @@
       <c r="N56" s="36"/>
       <c r="O56" s="26"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15">
       <c r="B57" s="27" t="s">
         <v>112</v>
       </c>
@@ -6299,7 +6345,7 @@
       <c r="N57" s="36"/>
       <c r="O57" s="26"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15">
       <c r="B58" s="27" t="s">
         <v>114</v>
       </c>
@@ -6335,7 +6381,7 @@
       <c r="N58" s="36"/>
       <c r="O58" s="26"/>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15">
       <c r="B59" s="27" t="s">
         <v>117</v>
       </c>
@@ -6371,7 +6417,7 @@
       <c r="N59" s="36"/>
       <c r="O59" s="26"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15">
       <c r="B60" s="27" t="s">
         <v>119</v>
       </c>
@@ -6407,7 +6453,7 @@
       <c r="N60" s="36"/>
       <c r="O60" s="26"/>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15">
       <c r="B61" s="27" t="s">
         <v>121</v>
       </c>
@@ -6443,7 +6489,7 @@
       <c r="N61" s="36"/>
       <c r="O61" s="26"/>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15">
       <c r="B62" s="27" t="s">
         <v>123</v>
       </c>
@@ -6479,7 +6525,7 @@
       <c r="N62" s="36"/>
       <c r="O62" s="26"/>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15">
       <c r="B63" s="27" t="s">
         <v>125</v>
       </c>
@@ -6515,7 +6561,7 @@
       <c r="N63" s="36"/>
       <c r="O63" s="26"/>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15">
       <c r="B64" s="27" t="s">
         <v>127</v>
       </c>
@@ -6551,7 +6597,7 @@
       <c r="N64" s="36"/>
       <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:15">
       <c r="B65" s="27" t="s">
         <v>130</v>
       </c>
@@ -6587,7 +6633,7 @@
       <c r="N65" s="36"/>
       <c r="O65" s="26"/>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15">
       <c r="B66" s="27" t="s">
         <v>132</v>
       </c>
@@ -6623,7 +6669,7 @@
       <c r="N66" s="36"/>
       <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15">
       <c r="B67" s="27" t="s">
         <v>134</v>
       </c>
@@ -6659,7 +6705,7 @@
       <c r="N67" s="36"/>
       <c r="O67" s="26"/>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15">
       <c r="B68" s="27" t="s">
         <v>136</v>
       </c>
@@ -6695,7 +6741,7 @@
       <c r="N68" s="36"/>
       <c r="O68" s="26"/>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15">
       <c r="B69" s="27" t="s">
         <v>138</v>
       </c>
@@ -6731,7 +6777,7 @@
       <c r="N69" s="36"/>
       <c r="O69" s="26"/>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15">
       <c r="B70" s="27" t="s">
         <v>140</v>
       </c>
@@ -6767,7 +6813,7 @@
       <c r="N70" s="36"/>
       <c r="O70" s="26"/>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15">
       <c r="B71" s="27" t="s">
         <v>143</v>
       </c>
@@ -6803,7 +6849,7 @@
       <c r="N71" s="36"/>
       <c r="O71" s="26"/>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15">
       <c r="B72" s="27" t="s">
         <v>145</v>
       </c>
@@ -6839,7 +6885,7 @@
       <c r="N72" s="36"/>
       <c r="O72" s="26"/>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15">
       <c r="B73" s="27" t="s">
         <v>147</v>
       </c>
@@ -6875,7 +6921,7 @@
       <c r="N73" s="36"/>
       <c r="O73" s="26"/>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15">
       <c r="B74" s="27" t="s">
         <v>149</v>
       </c>
@@ -6911,7 +6957,7 @@
       <c r="N74" s="36"/>
       <c r="O74" s="26"/>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15">
       <c r="B75" s="27" t="s">
         <v>151</v>
       </c>
@@ -6947,7 +6993,7 @@
       <c r="N75" s="36"/>
       <c r="O75" s="26"/>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15">
       <c r="B76" s="27" t="s">
         <v>153</v>
       </c>
@@ -6984,7 +7030,7 @@
       <c r="N76" s="36"/>
       <c r="O76" s="26"/>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15">
       <c r="B77" s="27" t="s">
         <v>156</v>
       </c>
@@ -7021,7 +7067,7 @@
       <c r="N77" s="36"/>
       <c r="O77" s="26"/>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15">
       <c r="B78" s="27" t="s">
         <v>158</v>
       </c>
@@ -7058,7 +7104,7 @@
       <c r="N78" s="36"/>
       <c r="O78" s="26"/>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15">
       <c r="B79" s="27" t="s">
         <v>160</v>
       </c>
@@ -7095,7 +7141,7 @@
       <c r="N79" s="36"/>
       <c r="O79" s="26"/>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15">
       <c r="B80" s="27" t="s">
         <v>162</v>
       </c>
@@ -7132,7 +7178,7 @@
       <c r="N80" s="36"/>
       <c r="O80" s="26"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15">
       <c r="B81" s="27" t="s">
         <v>164</v>
       </c>
@@ -7169,7 +7215,7 @@
       <c r="N81" s="36"/>
       <c r="O81" s="26"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15">
       <c r="B82" s="27" t="s">
         <v>166</v>
       </c>
@@ -7206,7 +7252,7 @@
       <c r="N82" s="36"/>
       <c r="O82" s="26"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15">
       <c r="B83" s="46" t="s">
         <v>168</v>
       </c>
@@ -7243,7 +7289,7 @@
       <c r="N83" s="36"/>
       <c r="O83" s="26"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15">
       <c r="B84" s="46" t="s">
         <v>172</v>
       </c>
@@ -7280,7 +7326,7 @@
       <c r="N84" s="36"/>
       <c r="O84" s="26"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15">
       <c r="B85" s="46" t="s">
         <v>173</v>
       </c>
@@ -7317,7 +7363,7 @@
       <c r="N85" s="55"/>
       <c r="O85" s="26"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15">
       <c r="B86" s="46" t="s">
         <v>176</v>
       </c>
@@ -7354,7 +7400,7 @@
       <c r="N86" s="55"/>
       <c r="O86" s="26"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15">
       <c r="B87" s="46" t="s">
         <v>178</v>
       </c>
@@ -7391,7 +7437,7 @@
       <c r="N87" s="55"/>
       <c r="O87" s="26"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15">
       <c r="B88" s="46" t="s">
         <v>180</v>
       </c>
@@ -7428,7 +7474,7 @@
       <c r="N88" s="55"/>
       <c r="O88" s="26"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15">
       <c r="B89" s="46" t="s">
         <v>182</v>
       </c>
@@ -7465,7 +7511,7 @@
       <c r="N89" s="55"/>
       <c r="O89" s="26"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:15">
       <c r="B90" s="46" t="s">
         <v>184</v>
       </c>
@@ -7502,7 +7548,7 @@
       <c r="N90" s="55"/>
       <c r="O90" s="26"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15">
       <c r="B91" s="46" t="s">
         <v>186</v>
       </c>
@@ -7539,7 +7585,7 @@
       <c r="N91" s="55"/>
       <c r="O91" s="26"/>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:15">
       <c r="B92" s="46" t="s">
         <v>189</v>
       </c>
@@ -7576,7 +7622,7 @@
       <c r="N92" s="55"/>
       <c r="O92" s="26"/>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15">
       <c r="B93" s="46" t="s">
         <v>191</v>
       </c>
@@ -7613,7 +7659,7 @@
       <c r="N93" s="55"/>
       <c r="O93" s="26"/>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15">
       <c r="B94" s="46" t="s">
         <v>193</v>
       </c>
@@ -7650,7 +7696,7 @@
       <c r="N94" s="55"/>
       <c r="O94" s="26"/>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15">
       <c r="B95" s="46" t="s">
         <v>195</v>
       </c>
@@ -7687,7 +7733,7 @@
       <c r="N95" s="55"/>
       <c r="O95" s="26"/>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15">
       <c r="B96" s="46" t="s">
         <v>197</v>
       </c>
@@ -7724,7 +7770,7 @@
       <c r="N96" s="55"/>
       <c r="O96" s="26"/>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:15">
       <c r="B97" s="46" t="s">
         <v>199</v>
       </c>
@@ -7761,7 +7807,7 @@
       <c r="N97" s="55"/>
       <c r="O97" s="26"/>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:15">
       <c r="B98" s="46" t="s">
         <v>202</v>
       </c>
@@ -7798,7 +7844,7 @@
       <c r="N98" s="55"/>
       <c r="O98" s="26"/>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:15">
       <c r="B99" s="46" t="s">
         <v>204</v>
       </c>
@@ -7835,7 +7881,7 @@
       <c r="N99" s="55"/>
       <c r="O99" s="26"/>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:15">
       <c r="B100" s="46" t="s">
         <v>207</v>
       </c>
@@ -7869,7 +7915,7 @@
       </c>
       <c r="L100" s="58"/>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:15">
       <c r="B101" s="46" t="s">
         <v>209</v>
       </c>
@@ -7904,7 +7950,7 @@
       <c r="L101" s="58"/>
       <c r="M101" s="54"/>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:15">
       <c r="B102" s="46" t="s">
         <v>211</v>
       </c>
@@ -7939,7 +7985,7 @@
       <c r="L102" s="58"/>
       <c r="M102" s="54"/>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:15">
       <c r="B103" s="46" t="s">
         <v>212</v>
       </c>
@@ -7974,7 +8020,7 @@
       <c r="L103" s="58"/>
       <c r="M103" s="54"/>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:15">
       <c r="B104" s="46" t="s">
         <v>216</v>
       </c>
@@ -8009,7 +8055,7 @@
       <c r="L104" s="58"/>
       <c r="M104" s="54"/>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:15">
       <c r="B105" s="46" t="s">
         <v>218</v>
       </c>
@@ -8044,7 +8090,7 @@
       <c r="L105" s="58"/>
       <c r="M105" s="54"/>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:15">
       <c r="B106" s="46" t="s">
         <v>220</v>
       </c>
@@ -8079,7 +8125,7 @@
       <c r="L106" s="58"/>
       <c r="M106" s="54"/>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:15">
       <c r="B107" s="46" t="s">
         <v>222</v>
       </c>
@@ -8114,7 +8160,7 @@
       <c r="L107" s="58"/>
       <c r="M107" s="54"/>
     </row>
-    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:15">
       <c r="B108" s="46" t="s">
         <v>225</v>
       </c>
@@ -8149,7 +8195,7 @@
       <c r="L108" s="58"/>
       <c r="M108" s="54"/>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:15">
       <c r="B109" s="46" t="s">
         <v>226</v>
       </c>
@@ -8184,7 +8230,7 @@
       <c r="L109" s="58"/>
       <c r="M109" s="54"/>
     </row>
-    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:15">
       <c r="B110" s="46" t="s">
         <v>228</v>
       </c>
@@ -8219,7 +8265,7 @@
       <c r="L110" s="58"/>
       <c r="M110" s="54"/>
     </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:15">
       <c r="B111" s="46" t="s">
         <v>231</v>
       </c>
@@ -8254,7 +8300,7 @@
       <c r="L111" s="58"/>
       <c r="M111" s="54"/>
     </row>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:15">
       <c r="B112" s="46" t="s">
         <v>233</v>
       </c>
@@ -8289,7 +8335,7 @@
       <c r="L112" s="58"/>
       <c r="M112" s="54"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:13">
       <c r="B113" s="46" t="s">
         <v>235</v>
       </c>
@@ -8324,7 +8370,7 @@
       <c r="L113" s="58"/>
       <c r="M113" s="54"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:13">
       <c r="B114" s="46" t="s">
         <v>237</v>
       </c>
@@ -8359,7 +8405,7 @@
       <c r="L114" s="58"/>
       <c r="M114" s="54"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:13">
       <c r="B115" s="46" t="s">
         <v>239</v>
       </c>
@@ -8394,7 +8440,7 @@
       <c r="L115" s="58"/>
       <c r="M115" s="54"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:13">
       <c r="B116" s="46" t="s">
         <v>242</v>
       </c>
@@ -8429,7 +8475,7 @@
       <c r="L116" s="58"/>
       <c r="M116" s="54"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:13">
       <c r="B117" s="46" t="s">
         <v>244</v>
       </c>
@@ -8464,7 +8510,7 @@
       <c r="L117" s="58"/>
       <c r="M117" s="54"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:13">
       <c r="B118" s="46" t="s">
         <v>246</v>
       </c>
@@ -8499,7 +8545,7 @@
       <c r="L118" s="58"/>
       <c r="M118" s="54"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:13">
       <c r="B119" s="46" t="s">
         <v>248</v>
       </c>
@@ -8534,7 +8580,7 @@
       <c r="L119" s="58"/>
       <c r="M119" s="54"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:13">
       <c r="B120" s="46" t="s">
         <v>250</v>
       </c>
@@ -8569,7 +8615,7 @@
       <c r="L120" s="58"/>
       <c r="M120" s="54"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:13">
       <c r="B121" s="46" t="s">
         <v>253</v>
       </c>
@@ -8604,7 +8650,7 @@
       <c r="L121" s="58"/>
       <c r="M121" s="54"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:13">
       <c r="B122" s="46" t="s">
         <v>255</v>
       </c>
@@ -8639,7 +8685,7 @@
       <c r="L122" s="58"/>
       <c r="M122" s="54"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:13">
       <c r="B123" s="46" t="s">
         <v>257</v>
       </c>
@@ -8674,7 +8720,7 @@
       <c r="L123" s="58"/>
       <c r="M123" s="54"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:13">
       <c r="B124" s="46" t="s">
         <v>259</v>
       </c>
@@ -8709,7 +8755,7 @@
       <c r="L124" s="58"/>
       <c r="M124" s="54"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:13">
       <c r="B125" s="46" t="s">
         <v>261</v>
       </c>
@@ -8744,7 +8790,7 @@
       <c r="L125" s="58"/>
       <c r="M125" s="54"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:13">
       <c r="B126" s="46" t="s">
         <v>263</v>
       </c>
@@ -8779,7 +8825,7 @@
       <c r="L126" s="58"/>
       <c r="M126" s="54"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:13">
       <c r="B127" s="46" t="s">
         <v>266</v>
       </c>
@@ -8814,7 +8860,7 @@
       <c r="L127" s="6"/>
       <c r="M127" s="60"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:13">
       <c r="B128" s="46" t="s">
         <v>269</v>
       </c>
@@ -8849,7 +8895,7 @@
       <c r="L128" s="6"/>
       <c r="M128" s="60"/>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:13">
       <c r="B129" s="46" t="s">
         <v>270</v>
       </c>
@@ -8884,7 +8930,7 @@
       <c r="L129" s="6"/>
       <c r="M129" s="60"/>
     </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:13">
       <c r="B130" s="46" t="s">
         <v>272</v>
       </c>
@@ -8919,7 +8965,7 @@
       <c r="L130" s="6"/>
       <c r="M130" s="60"/>
     </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:13">
       <c r="B131" s="46" t="s">
         <v>274</v>
       </c>
@@ -8954,7 +9000,7 @@
       <c r="L131" s="6"/>
       <c r="M131" s="60"/>
     </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:13">
       <c r="B132" s="46" t="s">
         <v>276</v>
       </c>
@@ -8989,7 +9035,7 @@
       <c r="L132" s="6"/>
       <c r="M132" s="60"/>
     </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:13">
       <c r="B133" s="46" t="s">
         <v>278</v>
       </c>
@@ -9024,7 +9070,7 @@
       <c r="L133" s="6"/>
       <c r="M133" s="60"/>
     </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:13">
       <c r="B134" s="46" t="s">
         <v>280</v>
       </c>
@@ -9059,7 +9105,7 @@
       <c r="L134" s="6"/>
       <c r="M134" s="60"/>
     </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:13">
       <c r="B135" s="46" t="s">
         <v>282</v>
       </c>
@@ -9094,7 +9140,7 @@
       <c r="L135" s="6"/>
       <c r="M135" s="60"/>
     </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:13">
       <c r="B136" s="46" t="s">
         <v>283</v>
       </c>
@@ -9129,7 +9175,7 @@
       <c r="L136" s="6"/>
       <c r="M136" s="60"/>
     </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:13">
       <c r="B137" s="46" t="s">
         <v>285</v>
       </c>
@@ -9164,7 +9210,7 @@
       <c r="L137" s="6"/>
       <c r="M137" s="60"/>
     </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:13">
       <c r="B138" s="46" t="s">
         <v>288</v>
       </c>
@@ -9199,7 +9245,7 @@
       <c r="L138" s="6"/>
       <c r="M138" s="60"/>
     </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:13">
       <c r="B139" s="46" t="s">
         <v>290</v>
       </c>
@@ -9234,7 +9280,7 @@
       <c r="L139" s="6"/>
       <c r="M139" s="60"/>
     </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:13">
       <c r="B140" s="46" t="s">
         <v>291</v>
       </c>
@@ -9269,7 +9315,7 @@
       <c r="L140" s="6"/>
       <c r="M140" s="60"/>
     </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:13">
       <c r="B141" s="46" t="s">
         <v>295</v>
       </c>
@@ -9304,7 +9350,7 @@
       <c r="L141" s="6"/>
       <c r="M141" s="60"/>
     </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:13">
       <c r="B142" s="46" t="s">
         <v>296</v>
       </c>
@@ -9339,7 +9385,7 @@
       <c r="L142" s="6"/>
       <c r="M142" s="60"/>
     </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:13">
       <c r="B143" s="46" t="s">
         <v>301</v>
       </c>
@@ -9374,7 +9420,7 @@
       <c r="L143" s="6"/>
       <c r="M143" s="60"/>
     </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:13">
       <c r="B144" s="46" t="s">
         <v>321</v>
       </c>
@@ -9409,7 +9455,7 @@
       <c r="L144" s="6"/>
       <c r="M144" s="60"/>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:13">
       <c r="B145" s="46" t="s">
         <v>327</v>
       </c>
@@ -9444,7 +9490,7 @@
       <c r="L145" s="6"/>
       <c r="M145" s="60"/>
     </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:13">
       <c r="B146" s="46" t="s">
         <v>328</v>
       </c>
@@ -9479,7 +9525,7 @@
       <c r="L146" s="6"/>
       <c r="M146" s="60"/>
     </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:13">
       <c r="B147" s="46" t="s">
         <v>330</v>
       </c>
@@ -9514,7 +9560,7 @@
       <c r="L147" s="6"/>
       <c r="M147" s="60"/>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:13">
       <c r="B148" s="46" t="s">
         <v>339</v>
       </c>
@@ -9548,7 +9594,7 @@
       <c r="L148" s="6"/>
       <c r="M148" s="60"/>
     </row>
-    <row r="149" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:13" ht="17" thickBot="1">
       <c r="B149" s="38" t="s">
         <v>335</v>
       </c>
@@ -9583,14 +9629,14 @@
       <c r="L149" s="6"/>
       <c r="M149" s="60"/>
     </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:13">
       <c r="B150" s="44"/>
       <c r="C150" s="44"/>
       <c r="D150" s="45"/>
       <c r="L150" s="6"/>
       <c r="M150" s="60"/>
     </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:13">
       <c r="B151" s="1" t="s">
         <v>170</v>
       </c>
@@ -9602,7 +9648,7 @@
       <c r="L151" s="59"/>
       <c r="M151" s="26"/>
     </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:13">
       <c r="F152" s="58"/>
       <c r="G152" s="26"/>
       <c r="H152" s="26"/>
@@ -9610,30 +9656,30 @@
       <c r="J152" s="26"/>
       <c r="K152" s="26"/>
     </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:13">
       <c r="G153" s="58"/>
       <c r="H153" s="68"/>
       <c r="K153" s="26"/>
     </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:13">
       <c r="E154" s="58"/>
       <c r="F154" s="58"/>
       <c r="G154" s="64"/>
       <c r="H154" s="58"/>
       <c r="K154" s="58"/>
     </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:13">
       <c r="G155" s="58"/>
       <c r="H155" s="64"/>
       <c r="I155" s="63"/>
       <c r="K155" s="58"/>
     </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:13">
       <c r="G156" s="58"/>
       <c r="H156" s="58"/>
       <c r="I156" s="58"/>
     </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:13">
       <c r="G157" s="58"/>
       <c r="J157" s="58"/>
     </row>
@@ -9647,7 +9693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -9658,26 +9704,26 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="2" style="6" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="6" customWidth="1"/>
-    <col min="5" max="6" width="19.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="19.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" style="6" customWidth="1"/>
     <col min="12" max="12" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="6"/>
+    <col min="13" max="13" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="C4" s="2" t="s">
         <v>309</v>
       </c>
@@ -9690,12 +9736,12 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="17" thickBot="1"/>
+    <row r="8" spans="2:14" ht="3.75" customHeight="1" thickBot="1">
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -9707,7 +9753,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:14" s="5" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" s="5" customFormat="1" ht="52" thickBot="1">
       <c r="B9" s="11" t="s">
         <v>0</v>
       </c>
@@ -9741,7 +9787,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" s="5" customFormat="1">
       <c r="B10" s="17" t="s">
         <v>4</v>
       </c>
@@ -9773,7 +9819,7 @@
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
     </row>
-    <row r="11" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" s="5" customFormat="1">
       <c r="B11" s="27" t="s">
         <v>7</v>
       </c>
@@ -9804,7 +9850,7 @@
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
     </row>
-    <row r="12" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" s="5" customFormat="1">
       <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
@@ -9835,7 +9881,7 @@
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
     </row>
-    <row r="13" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" s="5" customFormat="1">
       <c r="B13" s="27" t="s">
         <v>11</v>
       </c>
@@ -9866,7 +9912,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
     </row>
-    <row r="14" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" s="5" customFormat="1">
       <c r="B14" s="27" t="s">
         <v>13</v>
       </c>
@@ -9897,7 +9943,7 @@
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
     </row>
-    <row r="15" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" s="5" customFormat="1">
       <c r="B15" s="27" t="s">
         <v>15</v>
       </c>
@@ -9928,7 +9974,7 @@
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
     </row>
-    <row r="16" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" s="5" customFormat="1">
       <c r="B16" s="27" t="s">
         <v>17</v>
       </c>
@@ -9959,7 +10005,7 @@
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
     </row>
-    <row r="17" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" s="5" customFormat="1">
       <c r="B17" s="27" t="s">
         <v>20</v>
       </c>
@@ -9990,7 +10036,7 @@
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
     </row>
-    <row r="18" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" s="5" customFormat="1">
       <c r="B18" s="27" t="s">
         <v>22</v>
       </c>
@@ -10021,7 +10067,7 @@
       <c r="M18" s="26"/>
       <c r="N18" s="26"/>
     </row>
-    <row r="19" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" s="5" customFormat="1">
       <c r="B19" s="27" t="s">
         <v>24</v>
       </c>
@@ -10052,7 +10098,7 @@
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
     </row>
-    <row r="20" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" s="5" customFormat="1">
       <c r="B20" s="27" t="s">
         <v>27</v>
       </c>
@@ -10083,7 +10129,7 @@
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
     </row>
-    <row r="21" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" s="5" customFormat="1">
       <c r="B21" s="27" t="s">
         <v>29</v>
       </c>
@@ -10114,7 +10160,7 @@
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
     </row>
-    <row r="22" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" s="5" customFormat="1">
       <c r="B22" s="27" t="s">
         <v>32</v>
       </c>
@@ -10145,7 +10191,7 @@
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
     </row>
-    <row r="23" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" s="5" customFormat="1">
       <c r="B23" s="27" t="s">
         <v>35</v>
       </c>
@@ -10176,7 +10222,7 @@
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
     </row>
-    <row r="24" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" s="5" customFormat="1">
       <c r="B24" s="27" t="s">
         <v>37</v>
       </c>
@@ -10207,7 +10253,7 @@
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
     </row>
-    <row r="25" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" s="5" customFormat="1">
       <c r="B25" s="27" t="s">
         <v>39</v>
       </c>
@@ -10238,7 +10284,7 @@
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
     </row>
-    <row r="26" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" s="5" customFormat="1">
       <c r="B26" s="27" t="s">
         <v>41</v>
       </c>
@@ -10269,7 +10315,7 @@
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
     </row>
-    <row r="27" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" s="5" customFormat="1">
       <c r="B27" s="27" t="s">
         <v>43</v>
       </c>
@@ -10300,7 +10346,7 @@
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
     </row>
-    <row r="28" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" s="5" customFormat="1">
       <c r="B28" s="27" t="s">
         <v>45</v>
       </c>
@@ -10331,7 +10377,7 @@
       <c r="M28" s="26"/>
       <c r="N28" s="26"/>
     </row>
-    <row r="29" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" s="5" customFormat="1">
       <c r="B29" s="27" t="s">
         <v>48</v>
       </c>
@@ -10362,7 +10408,7 @@
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
     </row>
-    <row r="30" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" s="5" customFormat="1">
       <c r="B30" s="27" t="s">
         <v>50</v>
       </c>
@@ -10393,7 +10439,7 @@
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
     </row>
-    <row r="31" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" s="5" customFormat="1">
       <c r="B31" s="27" t="s">
         <v>52</v>
       </c>
@@ -10424,7 +10470,7 @@
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
     </row>
-    <row r="32" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" s="5" customFormat="1">
       <c r="B32" s="27" t="s">
         <v>54</v>
       </c>
@@ -10455,7 +10501,7 @@
       <c r="M32" s="26"/>
       <c r="N32" s="26"/>
     </row>
-    <row r="33" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" s="5" customFormat="1">
       <c r="B33" s="27" t="s">
         <v>57</v>
       </c>
@@ -10486,7 +10532,7 @@
       <c r="M33" s="26"/>
       <c r="N33" s="26"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15">
       <c r="B34" s="27" t="s">
         <v>59</v>
       </c>
@@ -10518,7 +10564,7 @@
       <c r="N34" s="26"/>
       <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15">
       <c r="B35" s="27" t="s">
         <v>62</v>
       </c>
@@ -10550,7 +10596,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15">
       <c r="B36" s="27" t="s">
         <v>65</v>
       </c>
@@ -10582,7 +10628,7 @@
       <c r="N36" s="26"/>
       <c r="O36" s="26"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15">
       <c r="B37" s="27" t="s">
         <v>67</v>
       </c>
@@ -10614,7 +10660,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="26"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15">
       <c r="B38" s="27" t="s">
         <v>69</v>
       </c>
@@ -10646,7 +10692,7 @@
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15">
       <c r="B39" s="27" t="s">
         <v>71</v>
       </c>
@@ -10678,7 +10724,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15">
       <c r="B40" s="27" t="s">
         <v>73</v>
       </c>
@@ -10710,7 +10756,7 @@
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15">
       <c r="B41" s="27" t="s">
         <v>76</v>
       </c>
@@ -10742,7 +10788,7 @@
       <c r="N41" s="26"/>
       <c r="O41" s="26"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15">
       <c r="B42" s="27" t="s">
         <v>78</v>
       </c>
@@ -10774,7 +10820,7 @@
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15">
       <c r="B43" s="27" t="s">
         <v>80</v>
       </c>
@@ -10806,7 +10852,7 @@
       <c r="N43" s="26"/>
       <c r="O43" s="26"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15">
       <c r="B44" s="27" t="s">
         <v>82</v>
       </c>
@@ -10838,7 +10884,7 @@
       <c r="N44" s="26"/>
       <c r="O44" s="26"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15">
       <c r="B45" s="27" t="s">
         <v>84</v>
       </c>
@@ -10870,7 +10916,7 @@
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15">
       <c r="B46" s="27" t="s">
         <v>86</v>
       </c>
@@ -10902,7 +10948,7 @@
       <c r="N46" s="26"/>
       <c r="O46" s="26"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15">
       <c r="B47" s="27" t="s">
         <v>89</v>
       </c>
@@ -10934,7 +10980,7 @@
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15">
       <c r="B48" s="27" t="s">
         <v>91</v>
       </c>
@@ -10966,7 +11012,7 @@
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15">
       <c r="B49" s="27" t="s">
         <v>93</v>
       </c>
@@ -10998,7 +11044,7 @@
       <c r="N49" s="26"/>
       <c r="O49" s="26"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15">
       <c r="B50" s="27" t="s">
         <v>95</v>
       </c>
@@ -11030,7 +11076,7 @@
       <c r="N50" s="26"/>
       <c r="O50" s="26"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15">
       <c r="B51" s="27" t="s">
         <v>97</v>
       </c>
@@ -11062,7 +11108,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="26"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15">
       <c r="B52" s="27" t="s">
         <v>100</v>
       </c>
@@ -11094,7 +11140,7 @@
       <c r="N52" s="26"/>
       <c r="O52" s="26"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15">
       <c r="B53" s="27" t="s">
         <v>103</v>
       </c>
@@ -11126,7 +11172,7 @@
       <c r="N53" s="26"/>
       <c r="O53" s="26"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15">
       <c r="B54" s="27" t="s">
         <v>105</v>
       </c>
@@ -11158,7 +11204,7 @@
       <c r="N54" s="36"/>
       <c r="O54" s="26"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15">
       <c r="B55" s="27" t="s">
         <v>107</v>
       </c>
@@ -11190,7 +11236,7 @@
       <c r="N55" s="36"/>
       <c r="O55" s="26"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15">
       <c r="B56" s="27" t="s">
         <v>109</v>
       </c>
@@ -11222,7 +11268,7 @@
       <c r="N56" s="36"/>
       <c r="O56" s="26"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15">
       <c r="B57" s="27" t="s">
         <v>112</v>
       </c>
@@ -11254,7 +11300,7 @@
       <c r="N57" s="36"/>
       <c r="O57" s="26"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15">
       <c r="B58" s="27" t="s">
         <v>114</v>
       </c>
@@ -11286,7 +11332,7 @@
       <c r="N58" s="36"/>
       <c r="O58" s="26"/>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15">
       <c r="B59" s="27" t="s">
         <v>117</v>
       </c>
@@ -11318,7 +11364,7 @@
       <c r="N59" s="36"/>
       <c r="O59" s="26"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15">
       <c r="B60" s="27" t="s">
         <v>119</v>
       </c>
@@ -11350,7 +11396,7 @@
       <c r="N60" s="36"/>
       <c r="O60" s="26"/>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15">
       <c r="B61" s="27" t="s">
         <v>121</v>
       </c>
@@ -11382,7 +11428,7 @@
       <c r="N61" s="36"/>
       <c r="O61" s="26"/>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15">
       <c r="B62" s="27" t="s">
         <v>123</v>
       </c>
@@ -11414,7 +11460,7 @@
       <c r="N62" s="36"/>
       <c r="O62" s="26"/>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15">
       <c r="B63" s="27" t="s">
         <v>125</v>
       </c>
@@ -11446,7 +11492,7 @@
       <c r="N63" s="36"/>
       <c r="O63" s="26"/>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15">
       <c r="B64" s="27" t="s">
         <v>127</v>
       </c>
@@ -11478,7 +11524,7 @@
       <c r="N64" s="36"/>
       <c r="O64" s="26"/>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:15">
       <c r="B65" s="27" t="s">
         <v>130</v>
       </c>
@@ -11510,7 +11556,7 @@
       <c r="N65" s="36"/>
       <c r="O65" s="26"/>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15">
       <c r="B66" s="27" t="s">
         <v>132</v>
       </c>
@@ -11542,7 +11588,7 @@
       <c r="N66" s="36"/>
       <c r="O66" s="26"/>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15">
       <c r="B67" s="27" t="s">
         <v>134</v>
       </c>
@@ -11574,7 +11620,7 @@
       <c r="N67" s="36"/>
       <c r="O67" s="26"/>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15">
       <c r="B68" s="27" t="s">
         <v>136</v>
       </c>
@@ -11606,7 +11652,7 @@
       <c r="N68" s="36"/>
       <c r="O68" s="26"/>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15">
       <c r="B69" s="27" t="s">
         <v>138</v>
       </c>
@@ -11638,7 +11684,7 @@
       <c r="N69" s="36"/>
       <c r="O69" s="26"/>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15">
       <c r="B70" s="27" t="s">
         <v>140</v>
       </c>
@@ -11670,7 +11716,7 @@
       <c r="N70" s="36"/>
       <c r="O70" s="26"/>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15">
       <c r="B71" s="27" t="s">
         <v>143</v>
       </c>
@@ -11702,7 +11748,7 @@
       <c r="N71" s="36"/>
       <c r="O71" s="26"/>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15">
       <c r="B72" s="27" t="s">
         <v>145</v>
       </c>
@@ -11734,7 +11780,7 @@
       <c r="N72" s="36"/>
       <c r="O72" s="26"/>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15">
       <c r="B73" s="27" t="s">
         <v>147</v>
       </c>
@@ -11766,7 +11812,7 @@
       <c r="N73" s="36"/>
       <c r="O73" s="26"/>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15">
       <c r="B74" s="27" t="s">
         <v>149</v>
       </c>
@@ -11798,7 +11844,7 @@
       <c r="N74" s="36"/>
       <c r="O74" s="26"/>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15">
       <c r="B75" s="27" t="s">
         <v>151</v>
       </c>
@@ -11834,7 +11880,7 @@
       <c r="N75" s="36"/>
       <c r="O75" s="26"/>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15">
       <c r="B76" s="27" t="s">
         <v>153</v>
       </c>
@@ -11870,7 +11916,7 @@
       <c r="N76" s="36"/>
       <c r="O76" s="26"/>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15">
       <c r="B77" s="27" t="s">
         <v>156</v>
       </c>
@@ -11906,7 +11952,7 @@
       <c r="N77" s="36"/>
       <c r="O77" s="26"/>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15">
       <c r="B78" s="27" t="s">
         <v>158</v>
       </c>
@@ -11942,7 +11988,7 @@
       <c r="N78" s="36"/>
       <c r="O78" s="26"/>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15">
       <c r="B79" s="27" t="s">
         <v>160</v>
       </c>
@@ -11978,7 +12024,7 @@
       <c r="N79" s="36"/>
       <c r="O79" s="26"/>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15">
       <c r="B80" s="27" t="s">
         <v>162</v>
       </c>
@@ -12014,7 +12060,7 @@
       <c r="N80" s="36"/>
       <c r="O80" s="26"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15">
       <c r="B81" s="27" t="s">
         <v>164</v>
       </c>
@@ -12050,7 +12096,7 @@
       <c r="N81" s="36"/>
       <c r="O81" s="26"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15">
       <c r="B82" s="27" t="s">
         <v>166</v>
       </c>
@@ -12086,7 +12132,7 @@
       <c r="N82" s="36"/>
       <c r="O82" s="26"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15">
       <c r="B83" s="46" t="s">
         <v>168</v>
       </c>
@@ -12122,7 +12168,7 @@
       <c r="N83" s="36"/>
       <c r="O83" s="26"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15">
       <c r="B84" s="46" t="s">
         <v>172</v>
       </c>
@@ -12158,7 +12204,7 @@
       <c r="N84" s="36"/>
       <c r="O84" s="26"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15">
       <c r="B85" s="46" t="s">
         <v>173</v>
       </c>
@@ -12194,7 +12240,7 @@
       <c r="N85" s="36"/>
       <c r="O85" s="26"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15">
       <c r="B86" s="46" t="s">
         <v>176</v>
       </c>
@@ -12231,7 +12277,7 @@
       <c r="N86" s="36"/>
       <c r="O86" s="26"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15">
       <c r="B87" s="46" t="s">
         <v>178</v>
       </c>
@@ -12268,7 +12314,7 @@
       <c r="N87" s="36"/>
       <c r="O87" s="26"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15">
       <c r="B88" s="46" t="s">
         <v>180</v>
       </c>
@@ -12305,7 +12351,7 @@
       <c r="N88" s="36"/>
       <c r="O88" s="26"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15">
       <c r="B89" s="46" t="s">
         <v>182</v>
       </c>
@@ -12342,7 +12388,7 @@
       <c r="N89" s="36"/>
       <c r="O89" s="26"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:15">
       <c r="B90" s="46" t="s">
         <v>184</v>
       </c>
@@ -12379,7 +12425,7 @@
       <c r="N90" s="36"/>
       <c r="O90" s="26"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15">
       <c r="B91" s="46" t="s">
         <v>186</v>
       </c>
@@ -12416,7 +12462,7 @@
       <c r="N91" s="36"/>
       <c r="O91" s="26"/>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:15">
       <c r="B92" s="46" t="s">
         <v>189</v>
       </c>
@@ -12453,7 +12499,7 @@
       <c r="N92" s="36"/>
       <c r="O92" s="26"/>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15">
       <c r="B93" s="46" t="s">
         <v>191</v>
       </c>
@@ -12490,7 +12536,7 @@
       <c r="N93" s="36"/>
       <c r="O93" s="26"/>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15">
       <c r="B94" s="46" t="s">
         <v>193</v>
       </c>
@@ -12527,7 +12573,7 @@
       <c r="N94" s="36"/>
       <c r="O94" s="26"/>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15">
       <c r="B95" s="46" t="s">
         <v>195</v>
       </c>
@@ -12564,7 +12610,7 @@
       <c r="N95" s="36"/>
       <c r="O95" s="26"/>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15">
       <c r="B96" s="46" t="s">
         <v>197</v>
       </c>
@@ -12601,7 +12647,7 @@
       <c r="N96" s="36"/>
       <c r="O96" s="26"/>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:15">
       <c r="B97" s="46" t="s">
         <v>199</v>
       </c>
@@ -12638,7 +12684,7 @@
       <c r="N97" s="36"/>
       <c r="O97" s="26"/>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:15">
       <c r="B98" s="46" t="s">
         <v>202</v>
       </c>
@@ -12675,7 +12721,7 @@
       <c r="N98" s="36"/>
       <c r="O98" s="26"/>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:15">
       <c r="B99" s="46" t="s">
         <v>204</v>
       </c>
@@ -12712,7 +12758,7 @@
       <c r="N99" s="36"/>
       <c r="O99" s="26"/>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:15">
       <c r="B100" s="46" t="s">
         <v>207</v>
       </c>
@@ -12747,7 +12793,7 @@
       <c r="L100" s="54"/>
       <c r="M100" s="26"/>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:15">
       <c r="B101" s="46" t="s">
         <v>209</v>
       </c>
@@ -12782,7 +12828,7 @@
       <c r="L101" s="54"/>
       <c r="M101" s="26"/>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:15">
       <c r="B102" s="46" t="s">
         <v>211</v>
       </c>
@@ -12817,7 +12863,7 @@
       <c r="L102" s="54"/>
       <c r="M102" s="26"/>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:15">
       <c r="B103" s="46" t="s">
         <v>212</v>
       </c>
@@ -12852,7 +12898,7 @@
       <c r="L103" s="54"/>
       <c r="M103" s="26"/>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:15">
       <c r="B104" s="46" t="s">
         <v>216</v>
       </c>
@@ -12889,7 +12935,7 @@
       <c r="L104" s="54"/>
       <c r="M104" s="26"/>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:15">
       <c r="B105" s="46" t="s">
         <v>218</v>
       </c>
@@ -12924,7 +12970,7 @@
       <c r="L105" s="54"/>
       <c r="M105" s="26"/>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:15">
       <c r="B106" s="46" t="s">
         <v>220</v>
       </c>
@@ -12959,7 +13005,7 @@
       <c r="L106" s="54"/>
       <c r="M106" s="26"/>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:15">
       <c r="B107" s="46" t="s">
         <v>222</v>
       </c>
@@ -12994,7 +13040,7 @@
       <c r="L107" s="54"/>
       <c r="M107" s="26"/>
     </row>
-    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:15">
       <c r="B108" s="46" t="s">
         <v>225</v>
       </c>
@@ -13029,7 +13075,7 @@
       <c r="L108" s="54"/>
       <c r="M108" s="26"/>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:15">
       <c r="B109" s="46" t="s">
         <v>226</v>
       </c>
@@ -13064,7 +13110,7 @@
       <c r="L109" s="54"/>
       <c r="M109" s="26"/>
     </row>
-    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:15">
       <c r="B110" s="46" t="s">
         <v>228</v>
       </c>
@@ -13099,7 +13145,7 @@
       <c r="L110" s="54"/>
       <c r="M110" s="26"/>
     </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:15">
       <c r="B111" s="46" t="s">
         <v>231</v>
       </c>
@@ -13134,7 +13180,7 @@
       <c r="L111" s="54"/>
       <c r="M111" s="26"/>
     </row>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:15">
       <c r="B112" s="46" t="s">
         <v>233</v>
       </c>
@@ -13169,7 +13215,7 @@
       <c r="L112" s="54"/>
       <c r="M112" s="26"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:13">
       <c r="B113" s="46" t="s">
         <v>235</v>
       </c>
@@ -13204,7 +13250,7 @@
       <c r="L113" s="54"/>
       <c r="M113" s="26"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:13">
       <c r="B114" s="46" t="s">
         <v>237</v>
       </c>
@@ -13239,7 +13285,7 @@
       <c r="L114" s="54"/>
       <c r="M114" s="26"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:13">
       <c r="B115" s="46" t="s">
         <v>239</v>
       </c>
@@ -13274,7 +13320,7 @@
       <c r="L115" s="54"/>
       <c r="M115" s="26"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:13">
       <c r="B116" s="46" t="s">
         <v>242</v>
       </c>
@@ -13309,7 +13355,7 @@
       <c r="L116" s="54"/>
       <c r="M116" s="26"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:13">
       <c r="B117" s="46" t="s">
         <v>244</v>
       </c>
@@ -13344,7 +13390,7 @@
       <c r="L117" s="54"/>
       <c r="M117" s="26"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:13">
       <c r="B118" s="46" t="s">
         <v>246</v>
       </c>
@@ -13379,7 +13425,7 @@
       <c r="L118" s="54"/>
       <c r="M118" s="26"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:13">
       <c r="B119" s="46" t="s">
         <v>248</v>
       </c>
@@ -13414,7 +13460,7 @@
       <c r="L119" s="54"/>
       <c r="M119" s="26"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:13">
       <c r="B120" s="46" t="s">
         <v>250</v>
       </c>
@@ -13449,7 +13495,7 @@
       <c r="L120" s="54"/>
       <c r="M120" s="26"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:13">
       <c r="B121" s="46" t="s">
         <v>253</v>
       </c>
@@ -13484,7 +13530,7 @@
       <c r="L121" s="54"/>
       <c r="M121" s="26"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:13">
       <c r="B122" s="46" t="s">
         <v>255</v>
       </c>
@@ -13519,7 +13565,7 @@
       <c r="L122" s="54"/>
       <c r="M122" s="26"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:13">
       <c r="B123" s="46" t="s">
         <v>298</v>
       </c>
@@ -13554,7 +13600,7 @@
       <c r="L123" s="54"/>
       <c r="M123" s="26"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:13">
       <c r="B124" s="46" t="s">
         <v>259</v>
       </c>
@@ -13589,7 +13635,7 @@
       <c r="L124" s="54"/>
       <c r="M124" s="26"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:13">
       <c r="B125" s="46" t="s">
         <v>261</v>
       </c>
@@ -13624,7 +13670,7 @@
       <c r="L125" s="54"/>
       <c r="M125" s="26"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:13">
       <c r="B126" s="46" t="s">
         <v>263</v>
       </c>
@@ -13659,7 +13705,7 @@
       <c r="L126" s="54"/>
       <c r="M126" s="26"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:13">
       <c r="B127" s="46" t="s">
         <v>266</v>
       </c>
@@ -13694,7 +13740,7 @@
       <c r="L127" s="54"/>
       <c r="M127" s="26"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:13">
       <c r="B128" s="46" t="s">
         <v>269</v>
       </c>
@@ -13729,7 +13775,7 @@
       <c r="L128" s="54"/>
       <c r="M128" s="26"/>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:13">
       <c r="B129" s="46" t="s">
         <v>270</v>
       </c>
@@ -13764,7 +13810,7 @@
       <c r="L129" s="54"/>
       <c r="M129" s="26"/>
     </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:13">
       <c r="B130" s="46" t="s">
         <v>272</v>
       </c>
@@ -13799,7 +13845,7 @@
       <c r="L130" s="54"/>
       <c r="M130" s="26"/>
     </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:13">
       <c r="B131" s="46" t="s">
         <v>274</v>
       </c>
@@ -13834,7 +13880,7 @@
       <c r="L131" s="54"/>
       <c r="M131" s="26"/>
     </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:13">
       <c r="B132" s="46" t="s">
         <v>276</v>
       </c>
@@ -13869,7 +13915,7 @@
       <c r="L132" s="54"/>
       <c r="M132" s="26"/>
     </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:13">
       <c r="B133" s="46" t="s">
         <v>278</v>
       </c>
@@ -13904,7 +13950,7 @@
       <c r="L133" s="54"/>
       <c r="M133" s="26"/>
     </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:13">
       <c r="B134" s="46" t="s">
         <v>280</v>
       </c>
@@ -13939,7 +13985,7 @@
       <c r="L134" s="54"/>
       <c r="M134" s="26"/>
     </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:13">
       <c r="B135" s="46" t="s">
         <v>282</v>
       </c>
@@ -13974,7 +14020,7 @@
       <c r="L135" s="54"/>
       <c r="M135" s="26"/>
     </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:13">
       <c r="B136" s="46" t="s">
         <v>283</v>
       </c>
@@ -14009,7 +14055,7 @@
       <c r="L136" s="54"/>
       <c r="M136" s="26"/>
     </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:13">
       <c r="B137" s="46" t="s">
         <v>285</v>
       </c>
@@ -14044,7 +14090,7 @@
       <c r="L137" s="54"/>
       <c r="M137" s="26"/>
     </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:13">
       <c r="B138" s="46" t="s">
         <v>288</v>
       </c>
@@ -14079,7 +14125,7 @@
       <c r="L138" s="54"/>
       <c r="M138" s="26"/>
     </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:13">
       <c r="B139" s="46" t="s">
         <v>290</v>
       </c>
@@ -14114,7 +14160,7 @@
       <c r="L139" s="54"/>
       <c r="M139" s="26"/>
     </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:13">
       <c r="B140" s="46" t="s">
         <v>291</v>
       </c>
@@ -14149,7 +14195,7 @@
       <c r="L140" s="54"/>
       <c r="M140" s="26"/>
     </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:13">
       <c r="B141" s="46" t="s">
         <v>295</v>
       </c>
@@ -14184,7 +14230,7 @@
       <c r="L141" s="54"/>
       <c r="M141" s="26"/>
     </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:13">
       <c r="B142" s="46" t="s">
         <v>296</v>
       </c>
@@ -14219,7 +14265,7 @@
       <c r="L142" s="54"/>
       <c r="M142" s="26"/>
     </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:13">
       <c r="B143" s="46" t="s">
         <v>301</v>
       </c>
@@ -14254,7 +14300,7 @@
       <c r="L143" s="54"/>
       <c r="M143" s="26"/>
     </row>
-    <row r="144" spans="2:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:13" s="72" customFormat="1">
       <c r="B144" s="46" t="s">
         <v>321</v>
       </c>
@@ -14289,7 +14335,7 @@
       <c r="L144" s="70"/>
       <c r="M144" s="71"/>
     </row>
-    <row r="145" spans="2:256" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:256" s="72" customFormat="1">
       <c r="B145" s="46" t="s">
         <v>327</v>
       </c>
@@ -14324,7 +14370,7 @@
       <c r="L145" s="70"/>
       <c r="M145" s="71"/>
     </row>
-    <row r="146" spans="2:256" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:256" s="72" customFormat="1">
       <c r="B146" s="46" t="s">
         <v>328</v>
       </c>
@@ -14359,7 +14405,7 @@
       <c r="L146" s="70"/>
       <c r="M146" s="71"/>
     </row>
-    <row r="147" spans="2:256" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:256" s="72" customFormat="1">
       <c r="B147" s="46" t="s">
         <v>330</v>
       </c>
@@ -14394,7 +14440,7 @@
       <c r="L147" s="70"/>
       <c r="M147" s="71"/>
     </row>
-    <row r="148" spans="2:256" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:256" s="72" customFormat="1">
       <c r="B148" s="46" t="s">
         <v>339</v>
       </c>
@@ -14428,7 +14474,7 @@
       <c r="L148" s="70"/>
       <c r="M148" s="71"/>
     </row>
-    <row r="149" spans="2:256" s="72" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:256" s="72" customFormat="1" ht="17" thickBot="1">
       <c r="B149" s="38" t="s">
         <v>335</v>
       </c>
@@ -14463,7 +14509,7 @@
       <c r="L149" s="70"/>
       <c r="M149" s="71"/>
     </row>
-    <row r="150" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:256">
       <c r="B150" s="44"/>
       <c r="C150" s="44"/>
       <c r="D150" s="44"/>
@@ -14720,30 +14766,30 @@
       <c r="IU150" s="44"/>
       <c r="IV150" s="44"/>
     </row>
-    <row r="151" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:256">
       <c r="B151" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I151" s="58"/>
       <c r="K151" s="67"/>
     </row>
-    <row r="152" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:256">
       <c r="G152" s="58"/>
       <c r="H152" s="68"/>
       <c r="I152" s="26"/>
     </row>
-    <row r="153" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:256">
       <c r="F153" s="58"/>
       <c r="H153" s="58"/>
       <c r="I153" s="68"/>
       <c r="J153" s="68"/>
     </row>
-    <row r="154" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:256">
       <c r="E154" s="58"/>
       <c r="F154" s="58"/>
       <c r="I154" s="58"/>
     </row>
-    <row r="155" spans="2:256" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:256">
       <c r="I155" s="58"/>
     </row>
   </sheetData>

</xml_diff>